<commit_message>
Enhanced UI/UX with comprehensive Help & Support system, quick actions integration, and refined Settings panel
</commit_message>
<xml_diff>
--- a/backend/output_timetables/sem1_CSE_timetable.xlsx
+++ b/backend/output_timetables/sem1_CSE_timetable.xlsx
@@ -472,27 +472,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>HS161</t>
+          <t>MA161</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>EC161</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>DS161</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>CS161</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>HS161</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>MA161</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>CS151 (Elective)</t>
         </is>
       </c>
     </row>
@@ -504,27 +504,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>CS151 (Elective)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>EC161</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>MA162</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>CS151 (Elective)</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>DS161</t>
-        </is>
-      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>EC161</t>
+          <t>MA162</t>
         </is>
       </c>
     </row>
@@ -568,27 +568,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>EC161</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>Free</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>CS151 (Elective)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
         <is>
           <t>HS161</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>EC161</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>CS161</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Free</t>
         </is>
       </c>
     </row>
@@ -600,22 +600,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>CS151 (Tutorial)</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Free</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -632,27 +632,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>MA162</t>
+          <t>CS161</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>HS161</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>MA161</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>HS161</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
           <t>DS161</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>MA161</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>CS161</t>
         </is>
       </c>
     </row>
@@ -742,27 +742,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>DS161</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>EC161</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>EC161</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>MA161</t>
-        </is>
-      </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>DS161</t>
+          <t>CS161</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>CS151 (Elective)</t>
+          <t>MA162</t>
         </is>
       </c>
     </row>
@@ -774,27 +774,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS151 (Elective)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MA162</t>
+          <t>HS161</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>CS151 (Elective)</t>
+          <t>CS161</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>EC161</t>
+          <t>HS161</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>MA162</t>
+          <t>HS161</t>
         </is>
       </c>
     </row>
@@ -838,7 +838,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CS161</t>
+          <t>MA161</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -848,17 +848,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS151 (Elective)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CS161</t>
+          <t>MA161</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>HS161</t>
+          <t>EC161</t>
         </is>
       </c>
     </row>
@@ -870,22 +870,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>CS151 (Tutorial)</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Free</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -902,27 +902,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>HS161</t>
+          <t>CS161</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>MA162</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>DS161</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>HS161</t>
-        </is>
-      </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>MA161</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>CS161</t>
+          <t>Free</t>
         </is>
       </c>
     </row>
@@ -3234,12 +3234,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Fri</t>
+          <t>Mon</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>09:00-10:30</t>
+          <t>10:30-12:00</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -3276,7 +3276,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>10:30-12:00</t>
+          <t>13:00-14:30</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -3308,7 +3308,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Mon</t>
+          <t>Thu</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">

</xml_diff>

<commit_message>
feat: implement comprehensive exam scheduling system with configurable constraints
</commit_message>
<xml_diff>
--- a/backend/output_timetables/sem1_CSE_timetable.xlsx
+++ b/backend/output_timetables/sem1_CSE_timetable.xlsx
@@ -472,27 +472,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MA161</t>
+          <t>CS151 (Elective)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>HS161</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>DS161</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>HS161</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>EC161</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>DS161</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>CS161</t>
         </is>
       </c>
     </row>
@@ -504,7 +504,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CS151 (Elective)</t>
+          <t>CS161</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -514,17 +514,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>CS161</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>MA162</t>
+          <t>EC161</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>MA162</t>
+          <t>Free</t>
         </is>
       </c>
     </row>
@@ -568,7 +568,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>EC161</t>
+          <t>MA161</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -578,17 +578,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>CS151 (Elective)</t>
+          <t>CS161</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA162</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>HS161</t>
+          <t>MA161</t>
         </is>
       </c>
     </row>
@@ -615,7 +615,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>CS151 (Tutorial)</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -632,27 +632,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>DS161</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>MA162</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>HS161</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>CS151 (Elective)</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
           <t>CS161</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>HS161</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>MA161</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>HS161</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>DS161</t>
         </is>
       </c>
     </row>
@@ -684,7 +684,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS151 (Tutorial)</t>
         </is>
       </c>
     </row>
@@ -742,27 +742,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>CS151 (Elective)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>DS161</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>EC161</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>EC161</t>
-        </is>
-      </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>CS161</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>MA162</t>
+          <t>HS161</t>
         </is>
       </c>
     </row>
@@ -774,27 +774,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CS151 (Elective)</t>
+          <t>MA161</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>HS161</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>HS161</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>CS161</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>HS161</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>HS161</t>
         </is>
       </c>
     </row>
@@ -838,27 +838,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>DS161</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>MA162</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>EC161</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>MA161</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>CS151 (Elective)</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>MA161</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>EC161</t>
         </is>
       </c>
     </row>
@@ -885,7 +885,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>CS151 (Tutorial)</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -902,22 +902,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>EC161</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>MA162</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>CS161</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>MA162</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>DS161</t>
-        </is>
-      </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS151 (Elective)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -954,7 +954,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS151 (Tutorial)</t>
         </is>
       </c>
     </row>
@@ -969,7 +969,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1023,6 +1023,11 @@
           <t>Instructor</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Department</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1042,7 +1047,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Branch: General</t>
+          <t>Department: CSE</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -1064,6 +1069,11 @@
           <t>Ramesh Athe</t>
         </is>
       </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1083,7 +1093,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Branch: General</t>
+          <t>Department: CSE</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -1105,6 +1115,11 @@
           <t>Abdul Wahid</t>
         </is>
       </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1124,7 +1139,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Branch: General</t>
+          <t>Department: CSE</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1146,6 +1161,11 @@
           <t>Chinmayananda</t>
         </is>
       </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1165,7 +1185,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Branch: General</t>
+          <t>Department: CSE</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1187,6 +1207,11 @@
           <t>Prakash Pawar</t>
         </is>
       </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1206,7 +1231,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Branch: General</t>
+          <t>Department: CSE</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1228,6 +1253,11 @@
           <t>Sunil P V, Sunil C K, Animesh Roy</t>
         </is>
       </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1247,7 +1277,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Branch: General</t>
+          <t>Department: CSE</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1269,6 +1299,11 @@
           <t>Rajesh N S</t>
         </is>
       </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1310,6 +1345,11 @@
           <t>Ravishankar, Vivekraj</t>
         </is>
       </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1351,6 +1391,11 @@
           <t>Vivekraj</t>
         </is>
       </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1392,6 +1437,11 @@
           <t>Mallikarjun Kande</t>
         </is>
       </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1433,6 +1483,11 @@
           <t>Chandrika Kamat</t>
         </is>
       </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1474,6 +1529,11 @@
           <t>Anand B</t>
         </is>
       </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1515,6 +1575,11 @@
           <t>Rajesh N S</t>
         </is>
       </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1556,6 +1621,11 @@
           <t>Sandesh Phalke</t>
         </is>
       </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1597,6 +1667,11 @@
           <t>Rajesh N S</t>
         </is>
       </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1638,26 +1713,31 @@
           <t>Girish Revadigar</t>
         </is>
       </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>MA161</t>
+          <t>PH151</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Statistics</t>
+          <t>Introduction to Physics</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Core</t>
+          <t>Elective</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Branch: General</t>
+          <t>Common for All Branches</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1676,29 +1756,34 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Ramesh Athe</t>
+          <t>Ravishankar</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>DSAI</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DS161</t>
+          <t>DS151</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Introduction to Programming</t>
+          <t>Linux for Engineers</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Core</t>
+          <t>Elective</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Branch: General</t>
+          <t>Common for All Branches</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1717,29 +1802,34 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Girish Revadigar</t>
+          <t>Vivekraj</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>DSAI</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>MA162</t>
+          <t>CS101</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Probability</t>
+          <t>Fundamentals of Computing</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Core</t>
+          <t>Elective</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Branch: General</t>
+          <t>Common for All Branches</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1758,142 +1848,162 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Chinmayananda</t>
+          <t>Mallikarjun K</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>DSAI</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>EC161</t>
+          <t>HS157</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Digital Design</t>
+          <t>Computational Thinking</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Core</t>
+          <t>Elective</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Branch: General</t>
+          <t>Common for All Branches</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>3-0-2-0-2</t>
+          <t>1-0-0-0-1</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G20" t="n">
         <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Prakash Pawar</t>
+          <t>Chandrika Ka...</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>DSAI</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>CS161</t>
+          <t>HS102</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Problem Solving</t>
+          <t>Kannada Kali-Nali</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Core</t>
+          <t>Elective</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Branch: General</t>
+          <t>Common for All Branches</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>3-0-2-0-4</t>
+          <t>2-0-0-0-2</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G21" t="n">
         <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Animesh Roy</t>
+          <t>Anand B</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>DSAI</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>C202</t>
+          <t>HS103</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Economics/IET</t>
+          <t>Leveraging IT for Better Life</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Core</t>
+          <t>Elective</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Branch: General</t>
+          <t>Common for All Branches</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>3-0-0-0-3</t>
+          <t>2-0-0-0-2</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G22" t="n">
         <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Anushree Kini</t>
+          <t>Rajesh N S</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>DSAI</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>PH151</t>
+          <t>DE101</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Introduction to Physics</t>
+          <t>Basics of Design</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1922,19 +2032,24 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Ravishankar</t>
+          <t>Sandesh Phalk...</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>DSAI</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>DS151</t>
+          <t>HS156</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Linux for Engineers</t>
+          <t>Holistic Personality Development</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1949,33 +2064,38 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2-0-0-0-2</t>
+          <t>1-0-0-0-1</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G24" t="n">
         <v>0</v>
       </c>
       <c r="H24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Vivekraj</t>
+          <t>Rajesh N S</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>DSAI</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>CS161</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Fundamentals of Computing</t>
+          <t>Introduction to C Programming</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -2004,19 +2124,24 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Mallikarjun K</t>
+          <t>Girish Revadigar</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>DSAI</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>HS157</t>
+          <t>PH151</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Computational Thinking</t>
+          <t>Introduction to Physics</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -2031,33 +2156,38 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1-0-0-0-1</t>
+          <t>2-0-0-0-2</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G26" t="n">
         <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Chandrika Ka...</t>
+          <t>Ravishankar</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>ECE</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>HS102</t>
+          <t>DS151</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Kannada Kali-Nali</t>
+          <t>Linux for Engineers</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -2086,19 +2216,24 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Anand B</t>
+          <t>Vivekraj</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>ECE</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>HS103</t>
+          <t>CS101</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Leveraging IT for Better Life</t>
+          <t>Fundamentals of Computing</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -2127,19 +2262,24 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Rajesh N S</t>
+          <t>Mallikarjun Kande</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>ECE</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>DE101</t>
+          <t>HS157</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Basics of Design</t>
+          <t>Computational Thinking</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -2154,33 +2294,38 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2-0-0-0-2</t>
+          <t>1-0-0-0-1</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G29" t="n">
         <v>0</v>
       </c>
       <c r="H29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Sandesh Phalk...</t>
+          <t>Chandrika Kamat</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>ECE</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>HS156</t>
+          <t>HS102</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Holistic Personality Development</t>
+          <t>Kannada Kali-Nali</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -2195,33 +2340,38 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1-0-0-0-1</t>
+          <t>2-0-0-0-2</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G30" t="n">
         <v>0</v>
       </c>
       <c r="H30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Rajesh N S</t>
+          <t>Anand B</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>ECE</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>CS161</t>
+          <t>HS103</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Introduction to C Programming</t>
+          <t>Leveraging IT for Better Life</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -2250,29 +2400,34 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Girish Revadigar</t>
+          <t>Rajesh N S</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>ECE</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>MA161</t>
+          <t>DE101</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Statistics</t>
+          <t>Basics of Design</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Core</t>
+          <t>Elective</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Branch: General</t>
+          <t>Common for All Branches</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -2291,70 +2446,80 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>Ramesh Athe</t>
+          <t>Sandesh Phalke</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>ECE</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>CS161</t>
+          <t>HS156</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Introduction to Programming</t>
+          <t>Holistic Personality Development</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Core</t>
+          <t>Elective</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Branch: General</t>
+          <t>Common for All Branches</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2-0-0-0-2</t>
+          <t>1-0-0-0-1</t>
         </is>
       </c>
       <c r="F33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G33" t="n">
         <v>0</v>
       </c>
       <c r="H33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>Girish Revadigar</t>
+          <t>Rajesh N S</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>ECE</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>MA162</t>
+          <t>CS161</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Probability</t>
+          <t>Introduction to C Programming</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Core</t>
+          <t>Elective</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Branch: General</t>
+          <t>Common for All Branches</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -2373,499 +2538,12 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>Chinmayananda</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>EC161</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Digital Design</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>Core</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>Branch: General</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>3-0-2-0-2</t>
-        </is>
-      </c>
-      <c r="F35" t="n">
-        <v>3</v>
-      </c>
-      <c r="G35" t="n">
-        <v>0</v>
-      </c>
-      <c r="H35" t="n">
-        <v>2</v>
-      </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>Prakash Pawar</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>CS161</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Problem Solving</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Core</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>Branch: General</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>3-0-2-0-4</t>
-        </is>
-      </c>
-      <c r="F36" t="n">
-        <v>3</v>
-      </c>
-      <c r="G36" t="n">
-        <v>0</v>
-      </c>
-      <c r="H36" t="n">
-        <v>4</v>
-      </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>Manjunath</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>C202</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Economics/IET</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>Core</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>Branch: General</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>3-0-0-0-3</t>
-        </is>
-      </c>
-      <c r="F37" t="n">
-        <v>3</v>
-      </c>
-      <c r="G37" t="n">
-        <v>0</v>
-      </c>
-      <c r="H37" t="n">
-        <v>3</v>
-      </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>PH151</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Introduction to Physics</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>Elective</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>Common for All Branches</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>2-0-0-0-2</t>
-        </is>
-      </c>
-      <c r="F38" t="n">
-        <v>2</v>
-      </c>
-      <c r="G38" t="n">
-        <v>0</v>
-      </c>
-      <c r="H38" t="n">
-        <v>2</v>
-      </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>Ravishankar</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>DS151</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Linux for Engineers</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>Elective</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>Common for All Branches</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>2-0-0-0-2</t>
-        </is>
-      </c>
-      <c r="F39" t="n">
-        <v>2</v>
-      </c>
-      <c r="G39" t="n">
-        <v>0</v>
-      </c>
-      <c r="H39" t="n">
-        <v>2</v>
-      </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>Vivekraj</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>CS101</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Fundamentals of Computing</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>Elective</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>Common for All Branches</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>2-0-0-0-2</t>
-        </is>
-      </c>
-      <c r="F40" t="n">
-        <v>2</v>
-      </c>
-      <c r="G40" t="n">
-        <v>0</v>
-      </c>
-      <c r="H40" t="n">
-        <v>2</v>
-      </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>Mallikarjun Kande</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>HS157</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>Computational Thinking</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>Elective</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>Common for All Branches</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>1-0-0-0-1</t>
-        </is>
-      </c>
-      <c r="F41" t="n">
-        <v>1</v>
-      </c>
-      <c r="G41" t="n">
-        <v>0</v>
-      </c>
-      <c r="H41" t="n">
-        <v>1</v>
-      </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>Chandrika Kamat</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>HS102</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Kannada Kali-Nali</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>Elective</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>Common for All Branches</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>2-0-0-0-2</t>
-        </is>
-      </c>
-      <c r="F42" t="n">
-        <v>2</v>
-      </c>
-      <c r="G42" t="n">
-        <v>0</v>
-      </c>
-      <c r="H42" t="n">
-        <v>2</v>
-      </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>Anand B</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>HS103</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>Leveraging IT for Better Life</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>Elective</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>Common for All Branches</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>2-0-0-0-2</t>
-        </is>
-      </c>
-      <c r="F43" t="n">
-        <v>2</v>
-      </c>
-      <c r="G43" t="n">
-        <v>0</v>
-      </c>
-      <c r="H43" t="n">
-        <v>2</v>
-      </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>Rajesh N S</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>DE101</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>Basics of Design</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>Elective</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>Common for All Branches</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>2-0-0-0-2</t>
-        </is>
-      </c>
-      <c r="F44" t="n">
-        <v>2</v>
-      </c>
-      <c r="G44" t="n">
-        <v>0</v>
-      </c>
-      <c r="H44" t="n">
-        <v>2</v>
-      </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>Sandesh Phalke</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>HS156</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>Holistic Personality Development</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>Elective</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>Common for All Branches</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>1-0-0-0-1</t>
-        </is>
-      </c>
-      <c r="F45" t="n">
-        <v>1</v>
-      </c>
-      <c r="G45" t="n">
-        <v>0</v>
-      </c>
-      <c r="H45" t="n">
-        <v>1</v>
-      </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>Rajesh N S</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>CS161</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>Introduction to C Programming</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Elective</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>Common for All Branches</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>2-0-0-0-2</t>
-        </is>
-      </c>
-      <c r="F46" t="n">
-        <v>2</v>
-      </c>
-      <c r="G46" t="n">
-        <v>0</v>
-      </c>
-      <c r="H46" t="n">
-        <v>2</v>
-      </c>
-      <c r="I46" t="inlineStr">
-        <is>
           <t>Girish Revadigar</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>ECE</t>
         </is>
       </c>
     </row>
@@ -3239,7 +2917,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>10:30-12:00</t>
+          <t>09:00-10:30</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -3271,12 +2949,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Wed</t>
+          <t>Thu</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>13:00-14:30</t>
+          <t>15:30-17:00</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -3308,12 +2986,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Thu</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>14:30-15:30</t>
+          <t>17:00-18:00</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">

</xml_diff>

<commit_message>
Auto-optimize exam scheduling: dynamically adjusts exams per slot (1-4) to guarantee all courses are scheduled within date range
</commit_message>
<xml_diff>
--- a/backend/output_timetables/sem1_CSE_timetable.xlsx
+++ b/backend/output_timetables/sem1_CSE_timetable.xlsx
@@ -472,27 +472,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CS151 (Elective)</t>
+          <t>DS161</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>HS161</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>MA161</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>DS161</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>HS161</t>
-        </is>
-      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>EC161</t>
+          <t>MA162</t>
         </is>
       </c>
     </row>
@@ -504,27 +504,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>MA161</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>CS161</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>EC161</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Free</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>EC161</t>
-        </is>
-      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS151 (Elective)</t>
         </is>
       </c>
     </row>
@@ -568,27 +568,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MA161</t>
+          <t>HS161</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>EC161</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>MA162</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>Free</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>CS161</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>MA162</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>MA161</t>
         </is>
       </c>
     </row>
@@ -632,27 +632,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>DS161</t>
+          <t>EC161</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>MA162</t>
+          <t>CS151 (Elective)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>HS161</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>CS151 (Elective)</t>
-        </is>
-      </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>CS161</t>
+          <t>HS161</t>
         </is>
       </c>
     </row>
@@ -742,27 +742,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CS151 (Elective)</t>
+          <t>EC161</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>DS161</t>
+          <t>EC161</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>EC161</t>
+          <t>MA161</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>HS161</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>HS161</t>
+          <t>CS161</t>
         </is>
       </c>
     </row>
@@ -774,27 +774,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>MA161</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>CS161</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>HS161</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>HS161</t>
-        </is>
-      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>CS161</t>
+          <t>CS151 (Elective)</t>
         </is>
       </c>
     </row>
@@ -838,27 +838,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>MA162</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>HS161</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>DS161</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>MA162</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>EC161</t>
-        </is>
-      </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>MA161</t>
+          <t>HS161</t>
         </is>
       </c>
     </row>
@@ -902,27 +902,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>DS161</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>CS151 (Elective)</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>EC161</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
         <is>
           <t>MA162</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>CS161</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>CS151 (Elective)</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Free</t>
         </is>
       </c>
     </row>
@@ -2912,12 +2912,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Mon</t>
+          <t>Tue</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>09:00-10:30</t>
+          <t>15:30-17:00</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -2949,12 +2949,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Thu</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>15:30-17:00</t>
+          <t>10:30-12:00</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">

</xml_diff>

<commit_message>
Implement basket-based elective scheduling with common time slots across all branches
</commit_message>
<xml_diff>
--- a/backend/output_timetables/sem1_CSE_timetable.xlsx
+++ b/backend/output_timetables/sem1_CSE_timetable.xlsx
@@ -469,12 +469,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>EC161</t>
+          <t>CS161</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CS161</t>
+          <t>HS161</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -484,7 +484,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>DS161</t>
+          <t>MA162</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -501,22 +501,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>MA161</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>HS161</t>
+          <t>CS161</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>CS161</t>
+          <t>EC161</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>MA161</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -565,27 +565,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>EC161</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA162</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>MA161</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>HS161</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>DS161</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>MA162</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>MA162</t>
         </is>
       </c>
     </row>
@@ -629,27 +629,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA161</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>DS161</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>EC161</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>EC161</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>HS161</t>
-        </is>
-      </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>CS161</t>
+          <t>Free</t>
         </is>
       </c>
     </row>
@@ -739,22 +739,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>EC161</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>MA162</t>
+          <t>HS161</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>HS161</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>CS161</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -771,22 +771,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>EC161</t>
+          <t>MA161</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>HS161</t>
+          <t>CS161</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>EC161</t>
+          <t>CS161</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>DS161</t>
+          <t>MA161</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -835,27 +835,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>DS161</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>HS161</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>EC161</t>
+          <t>MA162</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>CS161</t>
+          <t>MA162</t>
         </is>
       </c>
     </row>
@@ -899,27 +899,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>MA161</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>EC161</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>EC161</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>DS161</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>CS161</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>MA161</t>
-        </is>
-      </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>MA162</t>
+          <t>Free</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix: UI according to the new concise excel timetables
</commit_message>
<xml_diff>
--- a/backend/output_timetables/sem1_CSE_timetable.xlsx
+++ b/backend/output_timetables/sem1_CSE_timetable.xlsx
@@ -62,7 +62,7 @@
       <sz val="13"/>
     </font>
   </fonts>
-  <fills count="25">
+  <fills count="26">
     <fill>
       <patternFill/>
     </fill>
@@ -131,14 +131,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00b584e0"/>
-        <bgColor rgb="00b584e0"/>
+        <fgColor rgb="00FF6B6B"/>
+        <bgColor rgb="00FF6B6B"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00F2F2F2"/>
         <bgColor rgb="00F2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00b584e0"/>
+        <bgColor rgb="00b584e0"/>
       </patternFill>
     </fill>
     <fill>
@@ -240,18 +246,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -345,6 +351,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1250,7 +1259,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1263,7 +1272,8 @@
     <col width="14" customWidth="1" min="3" max="3"/>
     <col width="48" customWidth="1" min="4" max="4"/>
     <col width="27" customWidth="1" min="5" max="5"/>
-    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="24" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1297,6 +1307,7 @@
           <t>Fri</t>
         </is>
       </c>
+      <c r="G1" s="6" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="7" t="inlineStr">
@@ -1329,6 +1340,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G2" s="8" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="7" t="inlineStr">
@@ -1338,16 +1350,7 @@
       </c>
       <c r="B3" s="9" t="inlineStr">
         <is>
-          <t>PH151 [C202]
-DS151 [C203]
-CS101 [C204]
-CS151 [C205]
-HS157 [C302]
-HS102 [C303]
-HS103 [C304]
-DE101 [C305]
-HS156 [C102]
-HS152 [C104]</t>
+          <t>ELECTIVE_B1</t>
         </is>
       </c>
       <c r="C3" s="10" t="inlineStr">
@@ -1357,16 +1360,7 @@
       </c>
       <c r="D3" s="9" t="inlineStr">
         <is>
-          <t>PH151 [C202]
-DS151 [C203]
-CS101 [C204]
-CS151 [C205]
-HS157 [C302]
-HS102 [C303]
-HS103 [C304]
-DE101 [C305]
-HS156 [C102]
-HS152 [C104]</t>
+          <t>ELECTIVE_B1</t>
         </is>
       </c>
       <c r="E3" s="11" t="inlineStr">
@@ -1379,6 +1373,7 @@
           <t>HS161 [C202]</t>
         </is>
       </c>
+      <c r="G3" s="8" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="7" t="inlineStr">
@@ -1411,6 +1406,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G4" s="8" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="7" t="inlineStr">
@@ -1443,6 +1439,7 @@
           <t>LUNCH BREAK</t>
         </is>
       </c>
+      <c r="G5" s="8" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="7" t="inlineStr">
@@ -1462,7 +1459,7 @@
       </c>
       <c r="D6" s="14" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L105]</t>
+          <t>EC161 (Lab) [L206]</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -1475,6 +1472,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G6" s="8" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="7" t="inlineStr">
@@ -1494,7 +1492,7 @@
       </c>
       <c r="D7" s="14" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L105]</t>
+          <t>EC161 (Lab) [L206]</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1504,18 +1502,10 @@
       </c>
       <c r="F7" s="9" t="inlineStr">
         <is>
-          <t>PH151 (Tutorial) [C202]
-DS151 (Tutorial) [C203]
-CS101 (Tutorial) [C204]
-CS151 (Tutorial) [C205]
-HS157 (Tutorial) [C302]
-HS102 (Tutorial) [C303]
-HS103 (Tutorial) [C304]
-DE101 (Tutorial) [C305]
-HS156 (Tutorial) [C102]
-HS152 (Tutorial) [C104]</t>
-        </is>
-      </c>
+          <t>ELECTIVE_B1 (Tutorial)</t>
+        </is>
+      </c>
+      <c r="G7" s="8" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="7" t="inlineStr">
@@ -1548,6 +1538,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G8" s="8" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="7" t="inlineStr">
@@ -1580,6 +1571,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G9" s="8" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="7" t="inlineStr">
@@ -1612,6 +1604,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G10" s="8" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="7" t="n"/>
@@ -1620,6 +1613,7 @@
       <c r="D11" s="8" t="n"/>
       <c r="E11" s="8" t="n"/>
       <c r="F11" s="8" t="n"/>
+      <c r="G11" s="8" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="7" t="n"/>
@@ -1628,6 +1622,7 @@
       <c r="D12" s="8" t="n"/>
       <c r="E12" s="8" t="n"/>
       <c r="F12" s="8" t="n"/>
+      <c r="G12" s="8" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="17" t="inlineStr">
@@ -1640,6 +1635,7 @@
       <c r="D13" s="8" t="n"/>
       <c r="E13" s="8" t="n"/>
       <c r="F13" s="8" t="n"/>
+      <c r="G13" s="8" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="18" t="inlineStr">
@@ -1652,6 +1648,7 @@
       <c r="D14" s="8" t="n"/>
       <c r="E14" s="8" t="n"/>
       <c r="F14" s="8" t="n"/>
+      <c r="G14" s="8" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="19" t="inlineStr">
@@ -1674,8 +1671,21 @@
           <t>Term Type</t>
         </is>
       </c>
-      <c r="E15" s="8" t="n"/>
-      <c r="F15" s="8" t="n"/>
+      <c r="E15" s="20" t="inlineStr">
+        <is>
+          <t>Lectures Hrs</t>
+        </is>
+      </c>
+      <c r="F15" s="20" t="inlineStr">
+        <is>
+          <t>Tutorials Hrs</t>
+        </is>
+      </c>
+      <c r="G15" s="20" t="inlineStr">
+        <is>
+          <t>Labs Hrs</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="21" t="inlineStr">
@@ -1698,8 +1708,21 @@
           <t>Full Sem</t>
         </is>
       </c>
-      <c r="E16" s="8" t="n"/>
-      <c r="F16" s="8" t="n"/>
+      <c r="E16" s="8" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+      <c r="F16" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G16" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="22" t="inlineStr">
@@ -1722,8 +1745,21 @@
           <t>Pre-Mid Only</t>
         </is>
       </c>
-      <c r="E17" s="8" t="n"/>
-      <c r="F17" s="8" t="n"/>
+      <c r="E17" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+      <c r="F17" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G17" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="23" t="inlineStr">
@@ -1746,8 +1782,21 @@
           <t>Post-Mid Only</t>
         </is>
       </c>
-      <c r="E18" s="8" t="n"/>
-      <c r="F18" s="8" t="n"/>
+      <c r="E18" s="8" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+      <c r="F18" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G18" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="24" t="inlineStr">
@@ -1770,8 +1819,21 @@
           <t>Full Sem</t>
         </is>
       </c>
-      <c r="E19" s="8" t="n"/>
-      <c r="F19" s="8" t="n"/>
+      <c r="E19" s="8" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+      <c r="F19" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G19" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="25" t="inlineStr">
@@ -1794,8 +1856,21 @@
           <t>Pre-Mid Only</t>
         </is>
       </c>
-      <c r="E20" s="8" t="n"/>
-      <c r="F20" s="8" t="n"/>
+      <c r="E20" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+      <c r="F20" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G20" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="26" t="inlineStr">
@@ -1818,8 +1893,21 @@
           <t>Post-Mid Only</t>
         </is>
       </c>
-      <c r="E21" s="8" t="n"/>
-      <c r="F21" s="8" t="n"/>
+      <c r="E21" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+      <c r="F21" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G21" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="7" t="n"/>
@@ -1828,6 +1916,7 @@
       <c r="D22" s="8" t="n"/>
       <c r="E22" s="8" t="n"/>
       <c r="F22" s="8" t="n"/>
+      <c r="G22" s="8" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="18" t="inlineStr">
@@ -1840,6 +1929,7 @@
       <c r="D23" s="8" t="n"/>
       <c r="E23" s="8" t="n"/>
       <c r="F23" s="8" t="n"/>
+      <c r="G23" s="8" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="19" t="inlineStr">
@@ -1872,6 +1962,7 @@
           <t>L-T-P-S-C</t>
         </is>
       </c>
+      <c r="G24" s="8" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="7" t="inlineStr">
@@ -1884,14 +1975,14 @@
           <t>Introduction to quantam Physics</t>
         </is>
       </c>
-      <c r="C25" s="9" t="inlineStr">
+      <c r="C25" s="27" t="inlineStr">
         <is>
           <t>PH151</t>
         </is>
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C202], Wed 09:00-10:30 [C202]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E25" s="8" t="inlineStr">
@@ -1904,6 +1995,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G25" s="8" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="7" t="inlineStr">
@@ -1916,14 +2008,14 @@
           <t>Linux for Engineers</t>
         </is>
       </c>
-      <c r="C26" s="27" t="inlineStr">
+      <c r="C26" s="28" t="inlineStr">
         <is>
           <t>DS151</t>
         </is>
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C203], Wed 09:00-10:30 [C203]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E26" s="8" t="inlineStr">
@@ -1936,6 +2028,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G26" s="8" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="7" t="inlineStr">
@@ -1948,14 +2041,14 @@
           <t>Fundamentals of Computing</t>
         </is>
       </c>
-      <c r="C27" s="28" t="inlineStr">
+      <c r="C27" s="29" t="inlineStr">
         <is>
           <t>CS101</t>
         </is>
       </c>
       <c r="D27" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C204], Wed 09:00-10:30 [C204]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E27" s="8" t="inlineStr">
@@ -1968,6 +2061,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G27" s="8" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="7" t="inlineStr">
@@ -1980,14 +2074,14 @@
           <t>introduction to cyber security</t>
         </is>
       </c>
-      <c r="C28" s="29" t="inlineStr">
+      <c r="C28" s="30" t="inlineStr">
         <is>
           <t>CS151</t>
         </is>
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C205], Wed 09:00-10:30 [C205]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E28" s="8" t="inlineStr">
@@ -2000,6 +2094,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G28" s="8" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="7" t="inlineStr">
@@ -2012,14 +2107,14 @@
           <t>Computational musicology for hindustani music</t>
         </is>
       </c>
-      <c r="C29" s="30" t="inlineStr">
+      <c r="C29" s="31" t="inlineStr">
         <is>
           <t>HS157</t>
         </is>
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C302], Wed 09:00-10:30 [C302]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E29" s="8" t="inlineStr">
@@ -2032,6 +2127,7 @@
           <t>1-0-0-0-1</t>
         </is>
       </c>
+      <c r="G29" s="8" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="7" t="inlineStr">
@@ -2044,14 +2140,14 @@
           <t>Kannada Kali-Nali</t>
         </is>
       </c>
-      <c r="C30" s="31" t="inlineStr">
+      <c r="C30" s="32" t="inlineStr">
         <is>
           <t>HS102</t>
         </is>
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C303], Wed 09:00-10:30 [C303]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E30" s="8" t="inlineStr">
@@ -2064,6 +2160,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G30" s="8" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="7" t="inlineStr">
@@ -2076,14 +2173,14 @@
           <t>Leveraging IT for Better Life</t>
         </is>
       </c>
-      <c r="C31" s="32" t="inlineStr">
+      <c r="C31" s="33" t="inlineStr">
         <is>
           <t>HS103</t>
         </is>
       </c>
       <c r="D31" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C304], Wed 09:00-10:30 [C304]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E31" s="8" t="inlineStr">
@@ -2096,6 +2193,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G31" s="8" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="7" t="inlineStr">
@@ -2108,14 +2206,14 @@
           <t>Basics of Design</t>
         </is>
       </c>
-      <c r="C32" s="33" t="inlineStr">
+      <c r="C32" s="34" t="inlineStr">
         <is>
           <t>DE101</t>
         </is>
       </c>
       <c r="D32" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C305], Wed 09:00-10:30 [C305]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E32" s="8" t="inlineStr">
@@ -2128,6 +2226,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G32" s="8" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="7" t="inlineStr">
@@ -2140,14 +2239,14 @@
           <t>Holistic Personality Development</t>
         </is>
       </c>
-      <c r="C33" s="34" t="inlineStr">
+      <c r="C33" s="35" t="inlineStr">
         <is>
           <t>HS156</t>
         </is>
       </c>
       <c r="D33" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C102], Wed 09:00-10:30 [C102]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E33" s="8" t="inlineStr">
@@ -2160,6 +2259,7 @@
           <t>1-0-0-0-1</t>
         </is>
       </c>
+      <c r="G33" s="8" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="7" t="inlineStr">
@@ -2172,14 +2272,14 @@
           <t>Economics/IET</t>
         </is>
       </c>
-      <c r="C34" s="35" t="inlineStr">
+      <c r="C34" s="36" t="inlineStr">
         <is>
           <t>HS152</t>
         </is>
       </c>
       <c r="D34" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C104], Wed 09:00-10:30 [C104]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E34" s="8" t="inlineStr">
@@ -2192,10 +2292,11 @@
           <t>3-0-0-0-3</t>
         </is>
       </c>
+      <c r="G34" s="8" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A14:G14"/>
     <mergeCell ref="A23:F23"/>
     <mergeCell ref="A13:E13"/>
   </mergeCells>
@@ -2209,7 +2310,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2222,7 +2323,8 @@
     <col width="14" customWidth="1" min="3" max="3"/>
     <col width="48" customWidth="1" min="4" max="4"/>
     <col width="27" customWidth="1" min="5" max="5"/>
-    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="24" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2256,6 +2358,7 @@
           <t>Fri</t>
         </is>
       </c>
+      <c r="G1" s="6" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="7" t="inlineStr">
@@ -2288,6 +2391,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G2" s="8" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="7" t="inlineStr">
@@ -2297,35 +2401,17 @@
       </c>
       <c r="B3" s="9" t="inlineStr">
         <is>
-          <t>PH151 [C202]
-DS151 [C203]
-CS101 [C204]
-CS151 [C205]
-HS157 [C302]
-HS102 [C303]
-HS103 [C304]
-DE101 [C305]
-HS156 [C102]
-HS152 [C104]</t>
+          <t>ELECTIVE_B1</t>
         </is>
       </c>
       <c r="C3" s="10" t="inlineStr">
         <is>
-          <t>MA161 [C004]</t>
+          <t>MA161 [C003]</t>
         </is>
       </c>
       <c r="D3" s="9" t="inlineStr">
         <is>
-          <t>PH151 [C202]
-DS151 [C203]
-CS101 [C204]
-CS151 [C205]
-HS157 [C302]
-HS102 [C303]
-HS103 [C304]
-DE101 [C305]
-HS156 [C102]
-HS152 [C104]</t>
+          <t>ELECTIVE_B1</t>
         </is>
       </c>
       <c r="E3" s="11" t="inlineStr">
@@ -2338,6 +2424,7 @@
           <t>HS161 [C203]</t>
         </is>
       </c>
+      <c r="G3" s="8" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="7" t="inlineStr">
@@ -2347,17 +2434,17 @@
       </c>
       <c r="B4" s="10" t="inlineStr">
         <is>
-          <t>MA161 [C004]</t>
+          <t>MA161 [C003]</t>
         </is>
       </c>
       <c r="C4" s="13" t="inlineStr">
         <is>
-          <t>DS161 [C004]</t>
+          <t>DS161 [C003]</t>
         </is>
       </c>
       <c r="D4" s="14" t="inlineStr">
         <is>
-          <t>EC161 [C004]</t>
+          <t>EC161 [C003]</t>
         </is>
       </c>
       <c r="E4" s="12" t="inlineStr">
@@ -2370,6 +2457,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G4" s="8" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="7" t="inlineStr">
@@ -2402,6 +2490,7 @@
           <t>LUNCH BREAK</t>
         </is>
       </c>
+      <c r="G5" s="8" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="7" t="inlineStr">
@@ -2411,22 +2500,22 @@
       </c>
       <c r="B6" s="13" t="inlineStr">
         <is>
-          <t>DS161 [C004]</t>
+          <t>DS161 [C003]</t>
         </is>
       </c>
       <c r="C6" s="16" t="inlineStr">
         <is>
-          <t>MA162 [C004]</t>
+          <t>MA162 [C003]</t>
         </is>
       </c>
       <c r="D6" s="14" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L206]</t>
+          <t>EC161 (Lab) [L105]</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [L107]</t>
+          <t>CS161 (Lab) [L207]</t>
         </is>
       </c>
       <c r="F6" s="8" t="inlineStr">
@@ -2434,6 +2523,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G6" s="8" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="7" t="inlineStr">
@@ -2453,28 +2543,20 @@
       </c>
       <c r="D7" s="14" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L206]</t>
+          <t>EC161 (Lab) [L105]</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [L107]</t>
+          <t>CS161 (Lab) [L207]</t>
         </is>
       </c>
       <c r="F7" s="9" t="inlineStr">
         <is>
-          <t>PH151 (Tutorial) [C202]
-DS151 (Tutorial) [C203]
-CS101 (Tutorial) [C204]
-CS151 (Tutorial) [C205]
-HS157 (Tutorial) [C302]
-HS102 (Tutorial) [C303]
-HS103 (Tutorial) [C304]
-DE101 (Tutorial) [C305]
-HS156 (Tutorial) [C102]
-HS152 (Tutorial) [C104]</t>
-        </is>
-      </c>
+          <t>ELECTIVE_B1 (Tutorial)</t>
+        </is>
+      </c>
+      <c r="G7" s="8" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="7" t="inlineStr">
@@ -2484,12 +2566,12 @@
       </c>
       <c r="B8" s="16" t="inlineStr">
         <is>
-          <t>MA162 [C004]</t>
+          <t>MA162 [C003]</t>
         </is>
       </c>
       <c r="C8" s="14" t="inlineStr">
         <is>
-          <t>EC161 [C004]</t>
+          <t>EC161 [C003]</t>
         </is>
       </c>
       <c r="D8" s="11" t="inlineStr">
@@ -2507,6 +2589,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G8" s="8" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="7" t="inlineStr">
@@ -2539,6 +2622,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G9" s="8" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="7" t="inlineStr">
@@ -2571,6 +2655,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G10" s="8" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="7" t="n"/>
@@ -2579,6 +2664,7 @@
       <c r="D11" s="8" t="n"/>
       <c r="E11" s="8" t="n"/>
       <c r="F11" s="8" t="n"/>
+      <c r="G11" s="8" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="7" t="n"/>
@@ -2587,6 +2673,7 @@
       <c r="D12" s="8" t="n"/>
       <c r="E12" s="8" t="n"/>
       <c r="F12" s="8" t="n"/>
+      <c r="G12" s="8" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="17" t="inlineStr">
@@ -2599,6 +2686,7 @@
       <c r="D13" s="8" t="n"/>
       <c r="E13" s="8" t="n"/>
       <c r="F13" s="8" t="n"/>
+      <c r="G13" s="8" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="18" t="inlineStr">
@@ -2611,6 +2699,7 @@
       <c r="D14" s="8" t="n"/>
       <c r="E14" s="8" t="n"/>
       <c r="F14" s="8" t="n"/>
+      <c r="G14" s="8" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="19" t="inlineStr">
@@ -2633,8 +2722,21 @@
           <t>Term Type</t>
         </is>
       </c>
-      <c r="E15" s="8" t="n"/>
-      <c r="F15" s="8" t="n"/>
+      <c r="E15" s="20" t="inlineStr">
+        <is>
+          <t>Lectures Hrs</t>
+        </is>
+      </c>
+      <c r="F15" s="20" t="inlineStr">
+        <is>
+          <t>Tutorials Hrs</t>
+        </is>
+      </c>
+      <c r="G15" s="20" t="inlineStr">
+        <is>
+          <t>Labs Hrs</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="21" t="inlineStr">
@@ -2657,8 +2759,21 @@
           <t>Full Sem</t>
         </is>
       </c>
-      <c r="E16" s="8" t="n"/>
-      <c r="F16" s="8" t="n"/>
+      <c r="E16" s="8" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+      <c r="F16" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G16" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="22" t="inlineStr">
@@ -2681,8 +2796,21 @@
           <t>Pre-Mid Only</t>
         </is>
       </c>
-      <c r="E17" s="8" t="n"/>
-      <c r="F17" s="8" t="n"/>
+      <c r="E17" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+      <c r="F17" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G17" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="23" t="inlineStr">
@@ -2705,8 +2833,21 @@
           <t>Post-Mid Only</t>
         </is>
       </c>
-      <c r="E18" s="8" t="n"/>
-      <c r="F18" s="8" t="n"/>
+      <c r="E18" s="8" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+      <c r="F18" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G18" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="24" t="inlineStr">
@@ -2729,8 +2870,21 @@
           <t>Full Sem</t>
         </is>
       </c>
-      <c r="E19" s="8" t="n"/>
-      <c r="F19" s="8" t="n"/>
+      <c r="E19" s="8" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+      <c r="F19" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G19" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="25" t="inlineStr">
@@ -2753,8 +2907,21 @@
           <t>Pre-Mid Only</t>
         </is>
       </c>
-      <c r="E20" s="8" t="n"/>
-      <c r="F20" s="8" t="n"/>
+      <c r="E20" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+      <c r="F20" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G20" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="26" t="inlineStr">
@@ -2777,8 +2944,21 @@
           <t>Post-Mid Only</t>
         </is>
       </c>
-      <c r="E21" s="8" t="n"/>
-      <c r="F21" s="8" t="n"/>
+      <c r="E21" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+      <c r="F21" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G21" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="7" t="n"/>
@@ -2787,6 +2967,7 @@
       <c r="D22" s="8" t="n"/>
       <c r="E22" s="8" t="n"/>
       <c r="F22" s="8" t="n"/>
+      <c r="G22" s="8" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="18" t="inlineStr">
@@ -2799,6 +2980,7 @@
       <c r="D23" s="8" t="n"/>
       <c r="E23" s="8" t="n"/>
       <c r="F23" s="8" t="n"/>
+      <c r="G23" s="8" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="19" t="inlineStr">
@@ -2831,6 +3013,7 @@
           <t>L-T-P-S-C</t>
         </is>
       </c>
+      <c r="G24" s="8" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="7" t="inlineStr">
@@ -2843,14 +3026,14 @@
           <t>Introduction to quantam Physics</t>
         </is>
       </c>
-      <c r="C25" s="9" t="inlineStr">
+      <c r="C25" s="27" t="inlineStr">
         <is>
           <t>PH151</t>
         </is>
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C202], Wed 09:00-10:30 [C202]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E25" s="8" t="inlineStr">
@@ -2863,6 +3046,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G25" s="8" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="7" t="inlineStr">
@@ -2875,14 +3059,14 @@
           <t>Linux for Engineers</t>
         </is>
       </c>
-      <c r="C26" s="27" t="inlineStr">
+      <c r="C26" s="28" t="inlineStr">
         <is>
           <t>DS151</t>
         </is>
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C203], Wed 09:00-10:30 [C203]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E26" s="8" t="inlineStr">
@@ -2895,6 +3079,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G26" s="8" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="7" t="inlineStr">
@@ -2907,14 +3092,14 @@
           <t>Fundamentals of Computing</t>
         </is>
       </c>
-      <c r="C27" s="28" t="inlineStr">
+      <c r="C27" s="29" t="inlineStr">
         <is>
           <t>CS101</t>
         </is>
       </c>
       <c r="D27" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C204], Wed 09:00-10:30 [C204]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E27" s="8" t="inlineStr">
@@ -2927,6 +3112,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G27" s="8" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="7" t="inlineStr">
@@ -2939,14 +3125,14 @@
           <t>introduction to cyber security</t>
         </is>
       </c>
-      <c r="C28" s="29" t="inlineStr">
+      <c r="C28" s="30" t="inlineStr">
         <is>
           <t>CS151</t>
         </is>
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C205], Wed 09:00-10:30 [C205]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E28" s="8" t="inlineStr">
@@ -2959,6 +3145,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G28" s="8" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="7" t="inlineStr">
@@ -2971,14 +3158,14 @@
           <t>Computational musicology for hindustani music</t>
         </is>
       </c>
-      <c r="C29" s="30" t="inlineStr">
+      <c r="C29" s="31" t="inlineStr">
         <is>
           <t>HS157</t>
         </is>
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C302], Wed 09:00-10:30 [C302]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E29" s="8" t="inlineStr">
@@ -2991,6 +3178,7 @@
           <t>1-0-0-0-1</t>
         </is>
       </c>
+      <c r="G29" s="8" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="7" t="inlineStr">
@@ -3003,14 +3191,14 @@
           <t>Kannada Kali-Nali</t>
         </is>
       </c>
-      <c r="C30" s="31" t="inlineStr">
+      <c r="C30" s="32" t="inlineStr">
         <is>
           <t>HS102</t>
         </is>
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C303], Wed 09:00-10:30 [C303]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E30" s="8" t="inlineStr">
@@ -3023,6 +3211,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G30" s="8" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="7" t="inlineStr">
@@ -3035,14 +3224,14 @@
           <t>Leveraging IT for Better Life</t>
         </is>
       </c>
-      <c r="C31" s="32" t="inlineStr">
+      <c r="C31" s="33" t="inlineStr">
         <is>
           <t>HS103</t>
         </is>
       </c>
       <c r="D31" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C304], Wed 09:00-10:30 [C304]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E31" s="8" t="inlineStr">
@@ -3055,6 +3244,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G31" s="8" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="7" t="inlineStr">
@@ -3067,14 +3257,14 @@
           <t>Basics of Design</t>
         </is>
       </c>
-      <c r="C32" s="33" t="inlineStr">
+      <c r="C32" s="34" t="inlineStr">
         <is>
           <t>DE101</t>
         </is>
       </c>
       <c r="D32" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C305], Wed 09:00-10:30 [C305]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E32" s="8" t="inlineStr">
@@ -3087,6 +3277,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G32" s="8" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="7" t="inlineStr">
@@ -3099,14 +3290,14 @@
           <t>Holistic Personality Development</t>
         </is>
       </c>
-      <c r="C33" s="34" t="inlineStr">
+      <c r="C33" s="35" t="inlineStr">
         <is>
           <t>HS156</t>
         </is>
       </c>
       <c r="D33" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C102], Wed 09:00-10:30 [C102]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E33" s="8" t="inlineStr">
@@ -3119,6 +3310,7 @@
           <t>1-0-0-0-1</t>
         </is>
       </c>
+      <c r="G33" s="8" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="7" t="inlineStr">
@@ -3131,14 +3323,14 @@
           <t>Economics/IET</t>
         </is>
       </c>
-      <c r="C34" s="35" t="inlineStr">
+      <c r="C34" s="36" t="inlineStr">
         <is>
           <t>HS152</t>
         </is>
       </c>
       <c r="D34" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C104], Wed 09:00-10:30 [C104]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E34" s="8" t="inlineStr">
@@ -3151,10 +3343,11 @@
           <t>3-0-0-0-3</t>
         </is>
       </c>
+      <c r="G34" s="8" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A14:G14"/>
     <mergeCell ref="A23:F23"/>
     <mergeCell ref="A13:E13"/>
   </mergeCells>
@@ -3168,7 +3361,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3181,7 +3374,8 @@
     <col width="14" customWidth="1" min="3" max="3"/>
     <col width="48" customWidth="1" min="4" max="4"/>
     <col width="27" customWidth="1" min="5" max="5"/>
-    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="24" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3215,6 +3409,7 @@
           <t>Fri</t>
         </is>
       </c>
+      <c r="G1" s="6" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="7" t="inlineStr">
@@ -3247,6 +3442,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G2" s="8" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="7" t="inlineStr">
@@ -3254,16 +3450,9 @@
           <t>09:00-10:30</t>
         </is>
       </c>
-      <c r="B3" s="30" t="inlineStr">
-        <is>
-          <t>HS157 [C302]
-HS156 [C102]
-PH151 [C202]
-DS151 [C203]
-CS101 [C204]
-HS102 [C303]
-HS103 [C304]
-DE101 [C305]</t>
+      <c r="B3" s="9" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
@@ -3271,16 +3460,9 @@
           <t>CS161 [C202]</t>
         </is>
       </c>
-      <c r="D3" s="30" t="inlineStr">
-        <is>
-          <t>HS157 [C302]
-HS156 [C102]
-PH151 [C202]
-DS151 [C203]
-CS101 [C204]
-HS102 [C303]
-HS103 [C304]
-DE101 [C305]</t>
+      <c r="D3" s="9" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
         </is>
       </c>
       <c r="E3" s="8" t="inlineStr">
@@ -3293,6 +3475,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G3" s="8" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="7" t="inlineStr">
@@ -3312,7 +3495,7 @@
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>MA161 [C004]</t>
+          <t>MA161 [C003]</t>
         </is>
       </c>
       <c r="E4" s="8" t="inlineStr">
@@ -3325,6 +3508,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G4" s="8" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="7" t="inlineStr">
@@ -3357,6 +3541,7 @@
           <t>LUNCH BREAK</t>
         </is>
       </c>
+      <c r="G5" s="8" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="7" t="inlineStr">
@@ -3371,7 +3556,7 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>MA161 [C004]</t>
+          <t>MA161 [C003]</t>
         </is>
       </c>
       <c r="D6" s="13" t="inlineStr">
@@ -3389,6 +3574,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G6" s="8" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="7" t="inlineStr">
@@ -3416,18 +3602,12 @@
           <t>Free</t>
         </is>
       </c>
-      <c r="F7" s="30" t="inlineStr">
-        <is>
-          <t>HS157 (Tutorial) [C302]
-HS156 (Tutorial) [C102]
-PH151 (Tutorial) [C202]
-DS151 (Tutorial) [C203]
-CS101 (Tutorial) [C204]
-HS102 (Tutorial) [C303]
-HS103 (Tutorial) [C304]
-DE101 (Tutorial) [C305]</t>
-        </is>
-      </c>
+      <c r="F7" s="9" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1 (Tutorial)</t>
+        </is>
+      </c>
+      <c r="G7" s="8" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="7" t="inlineStr">
@@ -3442,7 +3622,7 @@
       </c>
       <c r="C8" s="13" t="inlineStr">
         <is>
-          <t>DS161 [C004]</t>
+          <t>DS161 [C003]</t>
         </is>
       </c>
       <c r="D8" s="8" t="inlineStr">
@@ -3460,6 +3640,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G8" s="8" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="7" t="inlineStr">
@@ -3492,6 +3673,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G9" s="8" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="7" t="inlineStr">
@@ -3524,6 +3706,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G10" s="8" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="7" t="n"/>
@@ -3532,6 +3715,7 @@
       <c r="D11" s="8" t="n"/>
       <c r="E11" s="8" t="n"/>
       <c r="F11" s="8" t="n"/>
+      <c r="G11" s="8" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="7" t="n"/>
@@ -3540,6 +3724,7 @@
       <c r="D12" s="8" t="n"/>
       <c r="E12" s="8" t="n"/>
       <c r="F12" s="8" t="n"/>
+      <c r="G12" s="8" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="17" t="inlineStr">
@@ -3552,6 +3737,7 @@
       <c r="D13" s="8" t="n"/>
       <c r="E13" s="8" t="n"/>
       <c r="F13" s="8" t="n"/>
+      <c r="G13" s="8" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="18" t="inlineStr">
@@ -3564,6 +3750,7 @@
       <c r="D14" s="8" t="n"/>
       <c r="E14" s="8" t="n"/>
       <c r="F14" s="8" t="n"/>
+      <c r="G14" s="8" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="19" t="inlineStr">
@@ -3586,8 +3773,21 @@
           <t>Term Type</t>
         </is>
       </c>
-      <c r="E15" s="8" t="n"/>
-      <c r="F15" s="8" t="n"/>
+      <c r="E15" s="20" t="inlineStr">
+        <is>
+          <t>Lectures Hrs</t>
+        </is>
+      </c>
+      <c r="F15" s="20" t="inlineStr">
+        <is>
+          <t>Tutorials Hrs</t>
+        </is>
+      </c>
+      <c r="G15" s="20" t="inlineStr">
+        <is>
+          <t>Labs Hrs</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="21" t="inlineStr">
@@ -3610,8 +3810,21 @@
           <t>Full Sem</t>
         </is>
       </c>
-      <c r="E16" s="8" t="n"/>
-      <c r="F16" s="8" t="n"/>
+      <c r="E16" s="8" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+      <c r="F16" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G16" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="22" t="inlineStr">
@@ -3634,8 +3847,21 @@
           <t>Pre-Mid Only</t>
         </is>
       </c>
-      <c r="E17" s="8" t="n"/>
-      <c r="F17" s="8" t="n"/>
+      <c r="E17" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+      <c r="F17" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G17" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="23" t="inlineStr">
@@ -3658,8 +3884,21 @@
           <t>Post-Mid Only</t>
         </is>
       </c>
-      <c r="E18" s="8" t="n"/>
-      <c r="F18" s="8" t="n"/>
+      <c r="E18" s="8" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+      <c r="F18" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G18" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="24" t="inlineStr">
@@ -3682,8 +3921,21 @@
           <t>Full Sem</t>
         </is>
       </c>
-      <c r="E19" s="8" t="n"/>
-      <c r="F19" s="8" t="n"/>
+      <c r="E19" s="8" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+      <c r="F19" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G19" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="25" t="inlineStr">
@@ -3706,8 +3958,21 @@
           <t>Pre-Mid Only</t>
         </is>
       </c>
-      <c r="E20" s="8" t="n"/>
-      <c r="F20" s="8" t="n"/>
+      <c r="E20" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+      <c r="F20" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G20" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="26" t="inlineStr">
@@ -3730,8 +3995,21 @@
           <t>Post-Mid Only</t>
         </is>
       </c>
-      <c r="E21" s="8" t="n"/>
-      <c r="F21" s="8" t="n"/>
+      <c r="E21" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+      <c r="F21" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G21" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="7" t="n"/>
@@ -3740,6 +4018,7 @@
       <c r="D22" s="8" t="n"/>
       <c r="E22" s="8" t="n"/>
       <c r="F22" s="8" t="n"/>
+      <c r="G22" s="8" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="18" t="inlineStr">
@@ -3752,6 +4031,7 @@
       <c r="D23" s="8" t="n"/>
       <c r="E23" s="8" t="n"/>
       <c r="F23" s="8" t="n"/>
+      <c r="G23" s="8" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="19" t="inlineStr">
@@ -3784,6 +4064,7 @@
           <t>L-T-P-S-C</t>
         </is>
       </c>
+      <c r="G24" s="8" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="7" t="inlineStr">
@@ -3796,14 +4077,14 @@
           <t>Introduction to quantam Physics</t>
         </is>
       </c>
-      <c r="C25" s="9" t="inlineStr">
+      <c r="C25" s="27" t="inlineStr">
         <is>
           <t>PH151</t>
         </is>
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C202], Wed 09:00-10:30 [C202]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E25" s="8" t="inlineStr">
@@ -3816,6 +4097,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G25" s="8" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="7" t="inlineStr">
@@ -3828,14 +4110,14 @@
           <t>Linux for Engineers</t>
         </is>
       </c>
-      <c r="C26" s="27" t="inlineStr">
+      <c r="C26" s="28" t="inlineStr">
         <is>
           <t>DS151</t>
         </is>
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C203], Wed 09:00-10:30 [C203]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E26" s="8" t="inlineStr">
@@ -3848,6 +4130,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G26" s="8" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="7" t="inlineStr">
@@ -3860,14 +4143,14 @@
           <t>Fundamentals of Computing</t>
         </is>
       </c>
-      <c r="C27" s="28" t="inlineStr">
+      <c r="C27" s="29" t="inlineStr">
         <is>
           <t>CS101</t>
         </is>
       </c>
       <c r="D27" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C204], Wed 09:00-10:30 [C204]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E27" s="8" t="inlineStr">
@@ -3880,6 +4163,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G27" s="8" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="7" t="inlineStr">
@@ -3892,14 +4176,14 @@
           <t>introduction to cyber security</t>
         </is>
       </c>
-      <c r="C28" s="29" t="inlineStr">
+      <c r="C28" s="30" t="inlineStr">
         <is>
           <t>CS151</t>
         </is>
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C205], Wed 09:00-10:30 [C205]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E28" s="8" t="inlineStr">
@@ -3912,6 +4196,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G28" s="8" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="7" t="inlineStr">
@@ -3924,14 +4209,14 @@
           <t>Computational musicology for hindustani music</t>
         </is>
       </c>
-      <c r="C29" s="30" t="inlineStr">
+      <c r="C29" s="31" t="inlineStr">
         <is>
           <t>HS157</t>
         </is>
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C302], Wed 09:00-10:30 [C302]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E29" s="8" t="inlineStr">
@@ -3944,6 +4229,7 @@
           <t>1-0-0-0-1</t>
         </is>
       </c>
+      <c r="G29" s="8" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="7" t="inlineStr">
@@ -3956,14 +4242,14 @@
           <t>Kannada Kali-Nali</t>
         </is>
       </c>
-      <c r="C30" s="31" t="inlineStr">
+      <c r="C30" s="32" t="inlineStr">
         <is>
           <t>HS102</t>
         </is>
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C303], Wed 09:00-10:30 [C303]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E30" s="8" t="inlineStr">
@@ -3976,6 +4262,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G30" s="8" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="7" t="inlineStr">
@@ -3988,14 +4275,14 @@
           <t>Leveraging IT for Better Life</t>
         </is>
       </c>
-      <c r="C31" s="32" t="inlineStr">
+      <c r="C31" s="33" t="inlineStr">
         <is>
           <t>HS103</t>
         </is>
       </c>
       <c r="D31" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C304], Wed 09:00-10:30 [C304]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E31" s="8" t="inlineStr">
@@ -4008,6 +4295,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G31" s="8" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="7" t="inlineStr">
@@ -4020,14 +4308,14 @@
           <t>Basics of Design</t>
         </is>
       </c>
-      <c r="C32" s="33" t="inlineStr">
+      <c r="C32" s="34" t="inlineStr">
         <is>
           <t>DE101</t>
         </is>
       </c>
       <c r="D32" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C305], Wed 09:00-10:30 [C305]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E32" s="8" t="inlineStr">
@@ -4040,6 +4328,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G32" s="8" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="7" t="inlineStr">
@@ -4052,14 +4341,14 @@
           <t>Holistic Personality Development</t>
         </is>
       </c>
-      <c r="C33" s="34" t="inlineStr">
+      <c r="C33" s="35" t="inlineStr">
         <is>
           <t>HS156</t>
         </is>
       </c>
       <c r="D33" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C102], Wed 09:00-10:30 [C102]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E33" s="8" t="inlineStr">
@@ -4072,6 +4361,7 @@
           <t>1-0-0-0-1</t>
         </is>
       </c>
+      <c r="G33" s="8" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="7" t="inlineStr">
@@ -4084,14 +4374,14 @@
           <t>Economics/IET</t>
         </is>
       </c>
-      <c r="C34" s="35" t="inlineStr">
+      <c r="C34" s="36" t="inlineStr">
         <is>
           <t>HS152</t>
         </is>
       </c>
       <c r="D34" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C104], Wed 09:00-10:30 [C104]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E34" s="8" t="inlineStr">
@@ -4104,10 +4394,11 @@
           <t>3-0-0-0-3</t>
         </is>
       </c>
+      <c r="G34" s="8" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A14:G14"/>
     <mergeCell ref="A23:F23"/>
     <mergeCell ref="A13:E13"/>
   </mergeCells>
@@ -4121,7 +4412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4134,7 +4425,8 @@
     <col width="14" customWidth="1" min="3" max="3"/>
     <col width="48" customWidth="1" min="4" max="4"/>
     <col width="27" customWidth="1" min="5" max="5"/>
-    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="24" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4168,6 +4460,7 @@
           <t>Fri</t>
         </is>
       </c>
+      <c r="G1" s="6" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="7" t="inlineStr">
@@ -4200,6 +4493,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G2" s="8" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="7" t="inlineStr">
@@ -4207,16 +4501,9 @@
           <t>09:00-10:30</t>
         </is>
       </c>
-      <c r="B3" s="30" t="inlineStr">
-        <is>
-          <t>HS157 [C302]
-HS156 [C102]
-PH151 [C202]
-DS151 [C203]
-CS101 [C204]
-HS102 [C303]
-HS103 [C304]
-DE101 [C305]</t>
+      <c r="B3" s="9" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
@@ -4224,16 +4511,9 @@
           <t>CS161 [C101]</t>
         </is>
       </c>
-      <c r="D3" s="30" t="inlineStr">
-        <is>
-          <t>HS157 [C302]
-HS156 [C102]
-PH151 [C202]
-DS151 [C203]
-CS101 [C204]
-HS102 [C303]
-HS103 [C304]
-DE101 [C305]</t>
+      <c r="D3" s="9" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
         </is>
       </c>
       <c r="E3" s="8" t="inlineStr">
@@ -4246,6 +4526,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G3" s="8" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="7" t="inlineStr">
@@ -4255,7 +4536,7 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>CS161 [C101]</t>
+          <t>CS161 [C102]</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
@@ -4265,7 +4546,7 @@
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>MA161 [C004]</t>
+          <t>MA161 [C003]</t>
         </is>
       </c>
       <c r="E4" s="8" t="inlineStr">
@@ -4278,6 +4559,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G4" s="8" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="7" t="inlineStr">
@@ -4310,6 +4592,7 @@
           <t>LUNCH BREAK</t>
         </is>
       </c>
+      <c r="G5" s="8" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="7" t="inlineStr">
@@ -4319,17 +4602,17 @@
       </c>
       <c r="B6" s="11" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [L207]</t>
+          <t>CS161 (Lab) [L106]</t>
         </is>
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>MA161 [C004]</t>
+          <t>MA161 [C003]</t>
         </is>
       </c>
       <c r="D6" s="13" t="inlineStr">
         <is>
-          <t>DS161 [C004]</t>
+          <t>DS161 [C003]</t>
         </is>
       </c>
       <c r="E6" s="8" t="inlineStr">
@@ -4342,6 +4625,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G6" s="8" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="7" t="inlineStr">
@@ -4351,7 +4635,7 @@
       </c>
       <c r="B7" s="11" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [L207]</t>
+          <t>CS161 (Lab) [L106]</t>
         </is>
       </c>
       <c r="C7" s="8" t="inlineStr">
@@ -4369,18 +4653,12 @@
           <t>Free</t>
         </is>
       </c>
-      <c r="F7" s="30" t="inlineStr">
-        <is>
-          <t>HS157 (Tutorial) [C302]
-HS156 (Tutorial) [C102]
-PH151 (Tutorial) [C202]
-DS151 (Tutorial) [C203]
-CS101 (Tutorial) [C204]
-HS102 (Tutorial) [C303]
-HS103 (Tutorial) [C304]
-DE101 (Tutorial) [C305]</t>
-        </is>
-      </c>
+      <c r="F7" s="9" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1 (Tutorial)</t>
+        </is>
+      </c>
+      <c r="G7" s="8" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="7" t="inlineStr">
@@ -4390,12 +4668,12 @@
       </c>
       <c r="B8" s="12" t="inlineStr">
         <is>
-          <t>HS161 [C101]</t>
+          <t>HS161 [C102]</t>
         </is>
       </c>
       <c r="C8" s="13" t="inlineStr">
         <is>
-          <t>DS161 [C004]</t>
+          <t>DS161 [C003]</t>
         </is>
       </c>
       <c r="D8" s="8" t="inlineStr">
@@ -4413,6 +4691,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G8" s="8" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="7" t="inlineStr">
@@ -4445,6 +4724,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G9" s="8" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="7" t="inlineStr">
@@ -4477,6 +4757,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G10" s="8" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="7" t="n"/>
@@ -4485,6 +4766,7 @@
       <c r="D11" s="8" t="n"/>
       <c r="E11" s="8" t="n"/>
       <c r="F11" s="8" t="n"/>
+      <c r="G11" s="8" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="7" t="n"/>
@@ -4493,6 +4775,7 @@
       <c r="D12" s="8" t="n"/>
       <c r="E12" s="8" t="n"/>
       <c r="F12" s="8" t="n"/>
+      <c r="G12" s="8" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="17" t="inlineStr">
@@ -4505,6 +4788,7 @@
       <c r="D13" s="8" t="n"/>
       <c r="E13" s="8" t="n"/>
       <c r="F13" s="8" t="n"/>
+      <c r="G13" s="8" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="18" t="inlineStr">
@@ -4517,6 +4801,7 @@
       <c r="D14" s="8" t="n"/>
       <c r="E14" s="8" t="n"/>
       <c r="F14" s="8" t="n"/>
+      <c r="G14" s="8" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="19" t="inlineStr">
@@ -4539,8 +4824,21 @@
           <t>Term Type</t>
         </is>
       </c>
-      <c r="E15" s="8" t="n"/>
-      <c r="F15" s="8" t="n"/>
+      <c r="E15" s="20" t="inlineStr">
+        <is>
+          <t>Lectures Hrs</t>
+        </is>
+      </c>
+      <c r="F15" s="20" t="inlineStr">
+        <is>
+          <t>Tutorials Hrs</t>
+        </is>
+      </c>
+      <c r="G15" s="20" t="inlineStr">
+        <is>
+          <t>Labs Hrs</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="21" t="inlineStr">
@@ -4563,8 +4861,21 @@
           <t>Full Sem</t>
         </is>
       </c>
-      <c r="E16" s="8" t="n"/>
-      <c r="F16" s="8" t="n"/>
+      <c r="E16" s="8" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+      <c r="F16" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G16" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="22" t="inlineStr">
@@ -4587,8 +4898,21 @@
           <t>Pre-Mid Only</t>
         </is>
       </c>
-      <c r="E17" s="8" t="n"/>
-      <c r="F17" s="8" t="n"/>
+      <c r="E17" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+      <c r="F17" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G17" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="23" t="inlineStr">
@@ -4611,8 +4935,21 @@
           <t>Post-Mid Only</t>
         </is>
       </c>
-      <c r="E18" s="8" t="n"/>
-      <c r="F18" s="8" t="n"/>
+      <c r="E18" s="8" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+      <c r="F18" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G18" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="24" t="inlineStr">
@@ -4635,8 +4972,21 @@
           <t>Full Sem</t>
         </is>
       </c>
-      <c r="E19" s="8" t="n"/>
-      <c r="F19" s="8" t="n"/>
+      <c r="E19" s="8" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+      <c r="F19" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G19" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="25" t="inlineStr">
@@ -4659,8 +5009,21 @@
           <t>Pre-Mid Only</t>
         </is>
       </c>
-      <c r="E20" s="8" t="n"/>
-      <c r="F20" s="8" t="n"/>
+      <c r="E20" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+      <c r="F20" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G20" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="26" t="inlineStr">
@@ -4683,8 +5046,21 @@
           <t>Post-Mid Only</t>
         </is>
       </c>
-      <c r="E21" s="8" t="n"/>
-      <c r="F21" s="8" t="n"/>
+      <c r="E21" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+      <c r="F21" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G21" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="7" t="n"/>
@@ -4693,6 +5069,7 @@
       <c r="D22" s="8" t="n"/>
       <c r="E22" s="8" t="n"/>
       <c r="F22" s="8" t="n"/>
+      <c r="G22" s="8" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="18" t="inlineStr">
@@ -4705,6 +5082,7 @@
       <c r="D23" s="8" t="n"/>
       <c r="E23" s="8" t="n"/>
       <c r="F23" s="8" t="n"/>
+      <c r="G23" s="8" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="19" t="inlineStr">
@@ -4737,6 +5115,7 @@
           <t>L-T-P-S-C</t>
         </is>
       </c>
+      <c r="G24" s="8" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="7" t="inlineStr">
@@ -4749,14 +5128,14 @@
           <t>Introduction to quantam Physics</t>
         </is>
       </c>
-      <c r="C25" s="9" t="inlineStr">
+      <c r="C25" s="27" t="inlineStr">
         <is>
           <t>PH151</t>
         </is>
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C202], Wed 09:00-10:30 [C202]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E25" s="8" t="inlineStr">
@@ -4769,6 +5148,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G25" s="8" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="7" t="inlineStr">
@@ -4781,14 +5161,14 @@
           <t>Linux for Engineers</t>
         </is>
       </c>
-      <c r="C26" s="27" t="inlineStr">
+      <c r="C26" s="28" t="inlineStr">
         <is>
           <t>DS151</t>
         </is>
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C203], Wed 09:00-10:30 [C203]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E26" s="8" t="inlineStr">
@@ -4801,6 +5181,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G26" s="8" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="7" t="inlineStr">
@@ -4813,14 +5194,14 @@
           <t>Fundamentals of Computing</t>
         </is>
       </c>
-      <c r="C27" s="28" t="inlineStr">
+      <c r="C27" s="29" t="inlineStr">
         <is>
           <t>CS101</t>
         </is>
       </c>
       <c r="D27" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C204], Wed 09:00-10:30 [C204]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E27" s="8" t="inlineStr">
@@ -4833,6 +5214,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G27" s="8" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="7" t="inlineStr">
@@ -4845,14 +5227,14 @@
           <t>introduction to cyber security</t>
         </is>
       </c>
-      <c r="C28" s="29" t="inlineStr">
+      <c r="C28" s="30" t="inlineStr">
         <is>
           <t>CS151</t>
         </is>
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C205], Wed 09:00-10:30 [C205]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E28" s="8" t="inlineStr">
@@ -4865,6 +5247,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G28" s="8" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="7" t="inlineStr">
@@ -4877,14 +5260,14 @@
           <t>Computational musicology for hindustani music</t>
         </is>
       </c>
-      <c r="C29" s="30" t="inlineStr">
+      <c r="C29" s="31" t="inlineStr">
         <is>
           <t>HS157</t>
         </is>
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C302], Wed 09:00-10:30 [C302]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E29" s="8" t="inlineStr">
@@ -4897,6 +5280,7 @@
           <t>1-0-0-0-1</t>
         </is>
       </c>
+      <c r="G29" s="8" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="7" t="inlineStr">
@@ -4909,14 +5293,14 @@
           <t>Kannada Kali-Nali</t>
         </is>
       </c>
-      <c r="C30" s="31" t="inlineStr">
+      <c r="C30" s="32" t="inlineStr">
         <is>
           <t>HS102</t>
         </is>
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C303], Wed 09:00-10:30 [C303]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E30" s="8" t="inlineStr">
@@ -4929,6 +5313,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G30" s="8" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="7" t="inlineStr">
@@ -4941,14 +5326,14 @@
           <t>Leveraging IT for Better Life</t>
         </is>
       </c>
-      <c r="C31" s="32" t="inlineStr">
+      <c r="C31" s="33" t="inlineStr">
         <is>
           <t>HS103</t>
         </is>
       </c>
       <c r="D31" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C304], Wed 09:00-10:30 [C304]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E31" s="8" t="inlineStr">
@@ -4961,6 +5346,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G31" s="8" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="7" t="inlineStr">
@@ -4973,14 +5359,14 @@
           <t>Basics of Design</t>
         </is>
       </c>
-      <c r="C32" s="33" t="inlineStr">
+      <c r="C32" s="34" t="inlineStr">
         <is>
           <t>DE101</t>
         </is>
       </c>
       <c r="D32" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C305], Wed 09:00-10:30 [C305]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E32" s="8" t="inlineStr">
@@ -4993,6 +5379,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G32" s="8" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="7" t="inlineStr">
@@ -5005,14 +5392,14 @@
           <t>Holistic Personality Development</t>
         </is>
       </c>
-      <c r="C33" s="34" t="inlineStr">
+      <c r="C33" s="35" t="inlineStr">
         <is>
           <t>HS156</t>
         </is>
       </c>
       <c r="D33" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C102], Wed 09:00-10:30 [C102]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E33" s="8" t="inlineStr">
@@ -5025,6 +5412,7 @@
           <t>1-0-0-0-1</t>
         </is>
       </c>
+      <c r="G33" s="8" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="7" t="inlineStr">
@@ -5037,14 +5425,14 @@
           <t>Economics/IET</t>
         </is>
       </c>
-      <c r="C34" s="35" t="inlineStr">
+      <c r="C34" s="36" t="inlineStr">
         <is>
           <t>HS152</t>
         </is>
       </c>
       <c r="D34" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C104], Wed 09:00-10:30 [C104]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E34" s="8" t="inlineStr">
@@ -5057,10 +5445,11 @@
           <t>3-0-0-0-3</t>
         </is>
       </c>
+      <c r="G34" s="8" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A14:G14"/>
     <mergeCell ref="A23:F23"/>
     <mergeCell ref="A13:E13"/>
   </mergeCells>
@@ -5074,7 +5463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5087,7 +5476,8 @@
     <col width="14" customWidth="1" min="3" max="3"/>
     <col width="48" customWidth="1" min="4" max="4"/>
     <col width="27" customWidth="1" min="5" max="5"/>
-    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="24" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5121,6 +5511,7 @@
           <t>Fri</t>
         </is>
       </c>
+      <c r="G1" s="6" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="7" t="inlineStr">
@@ -5153,6 +5544,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G2" s="8" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="7" t="inlineStr">
@@ -5160,11 +5552,9 @@
           <t>09:00-10:30</t>
         </is>
       </c>
-      <c r="B3" s="30" t="inlineStr">
-        <is>
-          <t>HS157 [C302]
-HS156 [C102]
-CS151 [C205]</t>
+      <c r="B3" s="9" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
@@ -5172,11 +5562,9 @@
           <t>CS161 [C102]</t>
         </is>
       </c>
-      <c r="D3" s="30" t="inlineStr">
-        <is>
-          <t>HS157 [C302]
-HS156 [C102]
-CS151 [C205]</t>
+      <c r="D3" s="9" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
         </is>
       </c>
       <c r="E3" s="8" t="inlineStr">
@@ -5189,6 +5577,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G3" s="8" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="7" t="inlineStr">
@@ -5198,7 +5587,7 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>CS161 [C102]</t>
+          <t>CS161 [C104]</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
@@ -5208,7 +5597,7 @@
       </c>
       <c r="D4" s="16" t="inlineStr">
         <is>
-          <t>MA162 [C004]</t>
+          <t>MA162 [C003]</t>
         </is>
       </c>
       <c r="E4" s="8" t="inlineStr">
@@ -5221,6 +5610,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G4" s="8" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="7" t="inlineStr">
@@ -5253,6 +5643,7 @@
           <t>LUNCH BREAK</t>
         </is>
       </c>
+      <c r="G5" s="8" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="7" t="inlineStr">
@@ -5262,17 +5653,17 @@
       </c>
       <c r="B6" s="11" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [L207]</t>
+          <t>CS161 (Lab) [L106]</t>
         </is>
       </c>
       <c r="C6" s="16" t="inlineStr">
         <is>
-          <t>MA162 [C004]</t>
+          <t>MA162 [C003]</t>
         </is>
       </c>
       <c r="D6" s="14" t="inlineStr">
         <is>
-          <t>EC161 [C004]</t>
+          <t>EC161 [C003]</t>
         </is>
       </c>
       <c r="E6" s="8" t="inlineStr">
@@ -5285,6 +5676,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G6" s="8" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="7" t="inlineStr">
@@ -5294,7 +5686,7 @@
       </c>
       <c r="B7" s="11" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [L207]</t>
+          <t>CS161 (Lab) [L106]</t>
         </is>
       </c>
       <c r="C7" s="8" t="inlineStr">
@@ -5312,13 +5704,12 @@
           <t>Free</t>
         </is>
       </c>
-      <c r="F7" s="30" t="inlineStr">
-        <is>
-          <t>HS157 (Tutorial) [C302]
-HS156 (Tutorial) [C102]
-CS151 (Tutorial) [C205]</t>
-        </is>
-      </c>
+      <c r="F7" s="9" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1 (Tutorial)</t>
+        </is>
+      </c>
+      <c r="G7" s="8" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="7" t="inlineStr">
@@ -5328,17 +5719,17 @@
       </c>
       <c r="B8" s="12" t="inlineStr">
         <is>
-          <t>HS161 [C102]</t>
+          <t>HS161 [C104]</t>
         </is>
       </c>
       <c r="C8" s="14" t="inlineStr">
         <is>
-          <t>EC161 [C004]</t>
+          <t>EC161 [C003]</t>
         </is>
       </c>
       <c r="D8" s="14" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L105]</t>
+          <t>EC161 (Lab) [L206]</t>
         </is>
       </c>
       <c r="E8" s="8" t="inlineStr">
@@ -5351,6 +5742,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G8" s="8" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="7" t="inlineStr">
@@ -5370,7 +5762,7 @@
       </c>
       <c r="D9" s="14" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L105]</t>
+          <t>EC161 (Lab) [L206]</t>
         </is>
       </c>
       <c r="E9" s="8" t="inlineStr">
@@ -5383,6 +5775,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G9" s="8" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="7" t="inlineStr">
@@ -5415,6 +5808,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G10" s="8" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="7" t="n"/>
@@ -5423,6 +5817,7 @@
       <c r="D11" s="8" t="n"/>
       <c r="E11" s="8" t="n"/>
       <c r="F11" s="8" t="n"/>
+      <c r="G11" s="8" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="7" t="n"/>
@@ -5431,6 +5826,7 @@
       <c r="D12" s="8" t="n"/>
       <c r="E12" s="8" t="n"/>
       <c r="F12" s="8" t="n"/>
+      <c r="G12" s="8" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="17" t="inlineStr">
@@ -5443,6 +5839,7 @@
       <c r="D13" s="8" t="n"/>
       <c r="E13" s="8" t="n"/>
       <c r="F13" s="8" t="n"/>
+      <c r="G13" s="8" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="18" t="inlineStr">
@@ -5455,6 +5852,7 @@
       <c r="D14" s="8" t="n"/>
       <c r="E14" s="8" t="n"/>
       <c r="F14" s="8" t="n"/>
+      <c r="G14" s="8" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="19" t="inlineStr">
@@ -5477,8 +5875,21 @@
           <t>Term Type</t>
         </is>
       </c>
-      <c r="E15" s="8" t="n"/>
-      <c r="F15" s="8" t="n"/>
+      <c r="E15" s="20" t="inlineStr">
+        <is>
+          <t>Lectures Hrs</t>
+        </is>
+      </c>
+      <c r="F15" s="20" t="inlineStr">
+        <is>
+          <t>Tutorials Hrs</t>
+        </is>
+      </c>
+      <c r="G15" s="20" t="inlineStr">
+        <is>
+          <t>Labs Hrs</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="21" t="inlineStr">
@@ -5501,8 +5912,21 @@
           <t>Full Sem</t>
         </is>
       </c>
-      <c r="E16" s="8" t="n"/>
-      <c r="F16" s="8" t="n"/>
+      <c r="E16" s="8" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+      <c r="F16" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G16" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="22" t="inlineStr">
@@ -5525,8 +5949,21 @@
           <t>Pre-Mid Only</t>
         </is>
       </c>
-      <c r="E17" s="8" t="n"/>
-      <c r="F17" s="8" t="n"/>
+      <c r="E17" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+      <c r="F17" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G17" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="23" t="inlineStr">
@@ -5549,8 +5986,21 @@
           <t>Post-Mid Only</t>
         </is>
       </c>
-      <c r="E18" s="8" t="n"/>
-      <c r="F18" s="8" t="n"/>
+      <c r="E18" s="8" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+      <c r="F18" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G18" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="24" t="inlineStr">
@@ -5573,8 +6023,21 @@
           <t>Full Sem</t>
         </is>
       </c>
-      <c r="E19" s="8" t="n"/>
-      <c r="F19" s="8" t="n"/>
+      <c r="E19" s="8" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+      <c r="F19" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G19" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="25" t="inlineStr">
@@ -5597,8 +6060,21 @@
           <t>Pre-Mid Only</t>
         </is>
       </c>
-      <c r="E20" s="8" t="n"/>
-      <c r="F20" s="8" t="n"/>
+      <c r="E20" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+      <c r="F20" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G20" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="26" t="inlineStr">
@@ -5621,8 +6097,21 @@
           <t>Post-Mid Only</t>
         </is>
       </c>
-      <c r="E21" s="8" t="n"/>
-      <c r="F21" s="8" t="n"/>
+      <c r="E21" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+      <c r="F21" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G21" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="7" t="n"/>
@@ -5631,6 +6120,7 @@
       <c r="D22" s="8" t="n"/>
       <c r="E22" s="8" t="n"/>
       <c r="F22" s="8" t="n"/>
+      <c r="G22" s="8" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="18" t="inlineStr">
@@ -5643,6 +6133,7 @@
       <c r="D23" s="8" t="n"/>
       <c r="E23" s="8" t="n"/>
       <c r="F23" s="8" t="n"/>
+      <c r="G23" s="8" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="19" t="inlineStr">
@@ -5675,6 +6166,7 @@
           <t>L-T-P-S-C</t>
         </is>
       </c>
+      <c r="G24" s="8" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="7" t="inlineStr">
@@ -5687,14 +6179,14 @@
           <t>Introduction to quantam Physics</t>
         </is>
       </c>
-      <c r="C25" s="9" t="inlineStr">
+      <c r="C25" s="27" t="inlineStr">
         <is>
           <t>PH151</t>
         </is>
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C202], Wed 09:00-10:30 [C202]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E25" s="8" t="inlineStr">
@@ -5707,6 +6199,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G25" s="8" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="7" t="inlineStr">
@@ -5719,14 +6212,14 @@
           <t>Linux for Engineers</t>
         </is>
       </c>
-      <c r="C26" s="27" t="inlineStr">
+      <c r="C26" s="28" t="inlineStr">
         <is>
           <t>DS151</t>
         </is>
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C203], Wed 09:00-10:30 [C203]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E26" s="8" t="inlineStr">
@@ -5739,6 +6232,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G26" s="8" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="7" t="inlineStr">
@@ -5751,14 +6245,14 @@
           <t>Fundamentals of Computing</t>
         </is>
       </c>
-      <c r="C27" s="28" t="inlineStr">
+      <c r="C27" s="29" t="inlineStr">
         <is>
           <t>CS101</t>
         </is>
       </c>
       <c r="D27" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C204], Wed 09:00-10:30 [C204]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E27" s="8" t="inlineStr">
@@ -5771,6 +6265,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G27" s="8" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="7" t="inlineStr">
@@ -5783,14 +6278,14 @@
           <t>introduction to cyber security</t>
         </is>
       </c>
-      <c r="C28" s="29" t="inlineStr">
+      <c r="C28" s="30" t="inlineStr">
         <is>
           <t>CS151</t>
         </is>
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C205], Wed 09:00-10:30 [C205]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E28" s="8" t="inlineStr">
@@ -5803,6 +6298,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G28" s="8" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="7" t="inlineStr">
@@ -5815,14 +6311,14 @@
           <t>Computational musicology for hindustani music</t>
         </is>
       </c>
-      <c r="C29" s="30" t="inlineStr">
+      <c r="C29" s="31" t="inlineStr">
         <is>
           <t>HS157</t>
         </is>
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C302], Wed 09:00-10:30 [C302]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E29" s="8" t="inlineStr">
@@ -5835,6 +6331,7 @@
           <t>1-0-0-0-1</t>
         </is>
       </c>
+      <c r="G29" s="8" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="7" t="inlineStr">
@@ -5847,14 +6344,14 @@
           <t>Kannada Kali-Nali</t>
         </is>
       </c>
-      <c r="C30" s="31" t="inlineStr">
+      <c r="C30" s="32" t="inlineStr">
         <is>
           <t>HS102</t>
         </is>
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C303], Wed 09:00-10:30 [C303]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E30" s="8" t="inlineStr">
@@ -5867,6 +6364,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G30" s="8" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="7" t="inlineStr">
@@ -5879,14 +6377,14 @@
           <t>Leveraging IT for Better Life</t>
         </is>
       </c>
-      <c r="C31" s="32" t="inlineStr">
+      <c r="C31" s="33" t="inlineStr">
         <is>
           <t>HS103</t>
         </is>
       </c>
       <c r="D31" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C304], Wed 09:00-10:30 [C304]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E31" s="8" t="inlineStr">
@@ -5899,6 +6397,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G31" s="8" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="7" t="inlineStr">
@@ -5911,14 +6410,14 @@
           <t>Basics of Design</t>
         </is>
       </c>
-      <c r="C32" s="33" t="inlineStr">
+      <c r="C32" s="34" t="inlineStr">
         <is>
           <t>DE101</t>
         </is>
       </c>
       <c r="D32" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C305], Wed 09:00-10:30 [C305]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E32" s="8" t="inlineStr">
@@ -5931,6 +6430,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G32" s="8" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="7" t="inlineStr">
@@ -5943,14 +6443,14 @@
           <t>Holistic Personality Development</t>
         </is>
       </c>
-      <c r="C33" s="34" t="inlineStr">
+      <c r="C33" s="35" t="inlineStr">
         <is>
           <t>HS156</t>
         </is>
       </c>
       <c r="D33" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C102], Wed 09:00-10:30 [C102]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E33" s="8" t="inlineStr">
@@ -5963,6 +6463,7 @@
           <t>1-0-0-0-1</t>
         </is>
       </c>
+      <c r="G33" s="8" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="7" t="inlineStr">
@@ -5975,14 +6476,14 @@
           <t>Economics/IET</t>
         </is>
       </c>
-      <c r="C34" s="35" t="inlineStr">
+      <c r="C34" s="36" t="inlineStr">
         <is>
           <t>HS152</t>
         </is>
       </c>
       <c r="D34" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C104], Wed 09:00-10:30 [C104]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E34" s="8" t="inlineStr">
@@ -5995,10 +6496,11 @@
           <t>3-0-0-0-3</t>
         </is>
       </c>
+      <c r="G34" s="8" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A14:G14"/>
     <mergeCell ref="A23:F23"/>
     <mergeCell ref="A13:E13"/>
   </mergeCells>
@@ -6012,7 +6514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6025,7 +6527,8 @@
     <col width="14" customWidth="1" min="3" max="3"/>
     <col width="48" customWidth="1" min="4" max="4"/>
     <col width="27" customWidth="1" min="5" max="5"/>
-    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="24" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6059,6 +6562,7 @@
           <t>Fri</t>
         </is>
       </c>
+      <c r="G1" s="6" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="7" t="inlineStr">
@@ -6091,6 +6595,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G2" s="8" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="7" t="inlineStr">
@@ -6098,11 +6603,9 @@
           <t>09:00-10:30</t>
         </is>
       </c>
-      <c r="B3" s="30" t="inlineStr">
-        <is>
-          <t>HS157 [C302]
-HS156 [C102]
-CS151 [C205]</t>
+      <c r="B3" s="9" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
@@ -6110,11 +6613,9 @@
           <t>CS161 [C104]</t>
         </is>
       </c>
-      <c r="D3" s="30" t="inlineStr">
-        <is>
-          <t>HS157 [C302]
-HS156 [C102]
-CS151 [C205]</t>
+      <c r="D3" s="9" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
         </is>
       </c>
       <c r="E3" s="8" t="inlineStr">
@@ -6127,6 +6628,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G3" s="8" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="7" t="inlineStr">
@@ -6136,7 +6638,7 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>CS161 [C104]</t>
+          <t>CS161 [C203]</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
@@ -6146,7 +6648,7 @@
       </c>
       <c r="D4" s="16" t="inlineStr">
         <is>
-          <t>MA162 [C004]</t>
+          <t>MA162 [C003]</t>
         </is>
       </c>
       <c r="E4" s="8" t="inlineStr">
@@ -6159,6 +6661,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G4" s="8" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="7" t="inlineStr">
@@ -6191,6 +6694,7 @@
           <t>LUNCH BREAK</t>
         </is>
       </c>
+      <c r="G5" s="8" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="7" t="inlineStr">
@@ -6200,17 +6704,17 @@
       </c>
       <c r="B6" s="11" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [L207]</t>
+          <t>CS161 (Lab) [L106]</t>
         </is>
       </c>
       <c r="C6" s="16" t="inlineStr">
         <is>
-          <t>MA162 [C004]</t>
+          <t>MA162 [C003]</t>
         </is>
       </c>
       <c r="D6" s="14" t="inlineStr">
         <is>
-          <t>EC161 [C004]</t>
+          <t>EC161 [C003]</t>
         </is>
       </c>
       <c r="E6" s="8" t="inlineStr">
@@ -6223,6 +6727,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G6" s="8" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="7" t="inlineStr">
@@ -6232,7 +6737,7 @@
       </c>
       <c r="B7" s="11" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [L207]</t>
+          <t>CS161 (Lab) [L106]</t>
         </is>
       </c>
       <c r="C7" s="8" t="inlineStr">
@@ -6250,13 +6755,12 @@
           <t>Free</t>
         </is>
       </c>
-      <c r="F7" s="30" t="inlineStr">
-        <is>
-          <t>HS157 (Tutorial) [C302]
-HS156 (Tutorial) [C102]
-CS151 (Tutorial) [C205]</t>
-        </is>
-      </c>
+      <c r="F7" s="9" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1 (Tutorial)</t>
+        </is>
+      </c>
+      <c r="G7" s="8" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="7" t="inlineStr">
@@ -6266,17 +6770,17 @@
       </c>
       <c r="B8" s="12" t="inlineStr">
         <is>
-          <t>HS161 [C104]</t>
+          <t>HS161 [C203]</t>
         </is>
       </c>
       <c r="C8" s="14" t="inlineStr">
         <is>
-          <t>EC161 [C004]</t>
+          <t>EC161 [C003]</t>
         </is>
       </c>
       <c r="D8" s="14" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L206]</t>
+          <t>EC161 (Lab) [L105]</t>
         </is>
       </c>
       <c r="E8" s="8" t="inlineStr">
@@ -6289,6 +6793,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G8" s="8" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="7" t="inlineStr">
@@ -6308,7 +6813,7 @@
       </c>
       <c r="D9" s="14" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L206]</t>
+          <t>EC161 (Lab) [L105]</t>
         </is>
       </c>
       <c r="E9" s="8" t="inlineStr">
@@ -6321,6 +6826,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G9" s="8" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="7" t="inlineStr">
@@ -6353,6 +6859,7 @@
           <t>Free</t>
         </is>
       </c>
+      <c r="G10" s="8" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="7" t="n"/>
@@ -6361,6 +6868,7 @@
       <c r="D11" s="8" t="n"/>
       <c r="E11" s="8" t="n"/>
       <c r="F11" s="8" t="n"/>
+      <c r="G11" s="8" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="7" t="n"/>
@@ -6369,6 +6877,7 @@
       <c r="D12" s="8" t="n"/>
       <c r="E12" s="8" t="n"/>
       <c r="F12" s="8" t="n"/>
+      <c r="G12" s="8" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="17" t="inlineStr">
@@ -6381,6 +6890,7 @@
       <c r="D13" s="8" t="n"/>
       <c r="E13" s="8" t="n"/>
       <c r="F13" s="8" t="n"/>
+      <c r="G13" s="8" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="18" t="inlineStr">
@@ -6393,6 +6903,7 @@
       <c r="D14" s="8" t="n"/>
       <c r="E14" s="8" t="n"/>
       <c r="F14" s="8" t="n"/>
+      <c r="G14" s="8" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="19" t="inlineStr">
@@ -6415,8 +6926,21 @@
           <t>Term Type</t>
         </is>
       </c>
-      <c r="E15" s="8" t="n"/>
-      <c r="F15" s="8" t="n"/>
+      <c r="E15" s="20" t="inlineStr">
+        <is>
+          <t>Lectures Hrs</t>
+        </is>
+      </c>
+      <c r="F15" s="20" t="inlineStr">
+        <is>
+          <t>Tutorials Hrs</t>
+        </is>
+      </c>
+      <c r="G15" s="20" t="inlineStr">
+        <is>
+          <t>Labs Hrs</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="21" t="inlineStr">
@@ -6439,8 +6963,21 @@
           <t>Full Sem</t>
         </is>
       </c>
-      <c r="E16" s="8" t="n"/>
-      <c r="F16" s="8" t="n"/>
+      <c r="E16" s="8" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+      <c r="F16" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G16" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="22" t="inlineStr">
@@ -6463,8 +7000,21 @@
           <t>Pre-Mid Only</t>
         </is>
       </c>
-      <c r="E17" s="8" t="n"/>
-      <c r="F17" s="8" t="n"/>
+      <c r="E17" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+      <c r="F17" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G17" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="23" t="inlineStr">
@@ -6487,8 +7037,21 @@
           <t>Post-Mid Only</t>
         </is>
       </c>
-      <c r="E18" s="8" t="n"/>
-      <c r="F18" s="8" t="n"/>
+      <c r="E18" s="8" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+      <c r="F18" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G18" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="24" t="inlineStr">
@@ -6511,8 +7074,21 @@
           <t>Full Sem</t>
         </is>
       </c>
-      <c r="E19" s="8" t="n"/>
-      <c r="F19" s="8" t="n"/>
+      <c r="E19" s="8" t="inlineStr">
+        <is>
+          <t>3/3</t>
+        </is>
+      </c>
+      <c r="F19" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G19" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="25" t="inlineStr">
@@ -6535,8 +7111,21 @@
           <t>Pre-Mid Only</t>
         </is>
       </c>
-      <c r="E20" s="8" t="n"/>
-      <c r="F20" s="8" t="n"/>
+      <c r="E20" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+      <c r="F20" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G20" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="26" t="inlineStr">
@@ -6559,8 +7148,21 @@
           <t>Post-Mid Only</t>
         </is>
       </c>
-      <c r="E21" s="8" t="n"/>
-      <c r="F21" s="8" t="n"/>
+      <c r="E21" s="8" t="inlineStr">
+        <is>
+          <t>2/2</t>
+        </is>
+      </c>
+      <c r="F21" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="G21" s="8" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="7" t="n"/>
@@ -6569,6 +7171,7 @@
       <c r="D22" s="8" t="n"/>
       <c r="E22" s="8" t="n"/>
       <c r="F22" s="8" t="n"/>
+      <c r="G22" s="8" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="18" t="inlineStr">
@@ -6581,6 +7184,7 @@
       <c r="D23" s="8" t="n"/>
       <c r="E23" s="8" t="n"/>
       <c r="F23" s="8" t="n"/>
+      <c r="G23" s="8" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="19" t="inlineStr">
@@ -6613,6 +7217,7 @@
           <t>L-T-P-S-C</t>
         </is>
       </c>
+      <c r="G24" s="8" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="7" t="inlineStr">
@@ -6625,14 +7230,14 @@
           <t>Introduction to quantam Physics</t>
         </is>
       </c>
-      <c r="C25" s="9" t="inlineStr">
+      <c r="C25" s="27" t="inlineStr">
         <is>
           <t>PH151</t>
         </is>
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C202], Wed 09:00-10:30 [C202]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E25" s="8" t="inlineStr">
@@ -6645,6 +7250,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G25" s="8" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="7" t="inlineStr">
@@ -6657,14 +7263,14 @@
           <t>Linux for Engineers</t>
         </is>
       </c>
-      <c r="C26" s="27" t="inlineStr">
+      <c r="C26" s="28" t="inlineStr">
         <is>
           <t>DS151</t>
         </is>
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C203], Wed 09:00-10:30 [C203]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E26" s="8" t="inlineStr">
@@ -6677,6 +7283,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G26" s="8" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="7" t="inlineStr">
@@ -6689,14 +7296,14 @@
           <t>Fundamentals of Computing</t>
         </is>
       </c>
-      <c r="C27" s="28" t="inlineStr">
+      <c r="C27" s="29" t="inlineStr">
         <is>
           <t>CS101</t>
         </is>
       </c>
       <c r="D27" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C204], Wed 09:00-10:30 [C204]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E27" s="8" t="inlineStr">
@@ -6709,6 +7316,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G27" s="8" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="7" t="inlineStr">
@@ -6721,14 +7329,14 @@
           <t>introduction to cyber security</t>
         </is>
       </c>
-      <c r="C28" s="29" t="inlineStr">
+      <c r="C28" s="30" t="inlineStr">
         <is>
           <t>CS151</t>
         </is>
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C205], Wed 09:00-10:30 [C205]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E28" s="8" t="inlineStr">
@@ -6741,6 +7349,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G28" s="8" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="7" t="inlineStr">
@@ -6753,14 +7362,14 @@
           <t>Computational musicology for hindustani music</t>
         </is>
       </c>
-      <c r="C29" s="30" t="inlineStr">
+      <c r="C29" s="31" t="inlineStr">
         <is>
           <t>HS157</t>
         </is>
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C302], Wed 09:00-10:30 [C302]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E29" s="8" t="inlineStr">
@@ -6773,6 +7382,7 @@
           <t>1-0-0-0-1</t>
         </is>
       </c>
+      <c r="G29" s="8" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="7" t="inlineStr">
@@ -6785,14 +7395,14 @@
           <t>Kannada Kali-Nali</t>
         </is>
       </c>
-      <c r="C30" s="31" t="inlineStr">
+      <c r="C30" s="32" t="inlineStr">
         <is>
           <t>HS102</t>
         </is>
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C303], Wed 09:00-10:30 [C303]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E30" s="8" t="inlineStr">
@@ -6805,6 +7415,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G30" s="8" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="7" t="inlineStr">
@@ -6817,14 +7428,14 @@
           <t>Leveraging IT for Better Life</t>
         </is>
       </c>
-      <c r="C31" s="32" t="inlineStr">
+      <c r="C31" s="33" t="inlineStr">
         <is>
           <t>HS103</t>
         </is>
       </c>
       <c r="D31" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C304], Wed 09:00-10:30 [C304]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E31" s="8" t="inlineStr">
@@ -6837,6 +7448,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G31" s="8" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="7" t="inlineStr">
@@ -6849,14 +7461,14 @@
           <t>Basics of Design</t>
         </is>
       </c>
-      <c r="C32" s="33" t="inlineStr">
+      <c r="C32" s="34" t="inlineStr">
         <is>
           <t>DE101</t>
         </is>
       </c>
       <c r="D32" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C305], Wed 09:00-10:30 [C305]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E32" s="8" t="inlineStr">
@@ -6869,6 +7481,7 @@
           <t>2-0-0-0-2</t>
         </is>
       </c>
+      <c r="G32" s="8" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="7" t="inlineStr">
@@ -6881,14 +7494,14 @@
           <t>Holistic Personality Development</t>
         </is>
       </c>
-      <c r="C33" s="34" t="inlineStr">
+      <c r="C33" s="35" t="inlineStr">
         <is>
           <t>HS156</t>
         </is>
       </c>
       <c r="D33" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C102], Wed 09:00-10:30 [C102]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E33" s="8" t="inlineStr">
@@ -6901,6 +7514,7 @@
           <t>1-0-0-0-1</t>
         </is>
       </c>
+      <c r="G33" s="8" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="7" t="inlineStr">
@@ -6913,14 +7527,14 @@
           <t>Economics/IET</t>
         </is>
       </c>
-      <c r="C34" s="35" t="inlineStr">
+      <c r="C34" s="36" t="inlineStr">
         <is>
           <t>HS152</t>
         </is>
       </c>
       <c r="D34" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C104], Wed 09:00-10:30 [C104]</t>
+          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
         </is>
       </c>
       <c r="E34" s="8" t="inlineStr">
@@ -6933,10 +7547,11 @@
           <t>3-0-0-0-3</t>
         </is>
       </c>
+      <c r="G34" s="8" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A14:G14"/>
     <mergeCell ref="A23:F23"/>
     <mergeCell ref="A13:E13"/>
   </mergeCells>

</xml_diff>

<commit_message>
Fix: Elective lecture and tutorial scheduling
</commit_message>
<xml_diff>
--- a/backend/output_timetables/sem1_CSE_timetable.xlsx
+++ b/backend/output_timetables/sem1_CSE_timetable.xlsx
@@ -1459,7 +1459,7 @@
       </c>
       <c r="D6" s="14" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L206]</t>
+          <t>EC161 (Lab) [L105]</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -1492,7 +1492,7 @@
       </c>
       <c r="D7" s="14" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L206]</t>
+          <t>EC161 (Lab) [L105]</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -1987,7 +1987,7 @@
       </c>
       <c r="E25" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C101]</t>
         </is>
       </c>
       <c r="F25" s="8" t="inlineStr">
@@ -2015,12 +2015,12 @@
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C102], Wed 09:00-10:30 [C102]</t>
         </is>
       </c>
       <c r="E26" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C102]</t>
         </is>
       </c>
       <c r="F26" s="8" t="inlineStr">
@@ -2048,12 +2048,12 @@
       </c>
       <c r="D27" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C104], Wed 09:00-10:30 [C104]</t>
         </is>
       </c>
       <c r="E27" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C104]</t>
         </is>
       </c>
       <c r="F27" s="8" t="inlineStr">
@@ -2081,12 +2081,12 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C202], Wed 09:00-10:30 [C202]</t>
         </is>
       </c>
       <c r="E28" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C202]</t>
         </is>
       </c>
       <c r="F28" s="8" t="inlineStr">
@@ -2114,12 +2114,12 @@
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C203], Wed 09:00-10:30 [C203]</t>
         </is>
       </c>
       <c r="E29" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C203]</t>
         </is>
       </c>
       <c r="F29" s="8" t="inlineStr">
@@ -2147,12 +2147,12 @@
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C204], Wed 09:00-10:30 [C204]</t>
         </is>
       </c>
       <c r="E30" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C204]</t>
         </is>
       </c>
       <c r="F30" s="8" t="inlineStr">
@@ -2180,12 +2180,12 @@
       </c>
       <c r="D31" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C205], Wed 09:00-10:30 [C205]</t>
         </is>
       </c>
       <c r="E31" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C205]</t>
         </is>
       </c>
       <c r="F31" s="8" t="inlineStr">
@@ -2213,12 +2213,12 @@
       </c>
       <c r="D32" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C302], Wed 09:00-10:30 [C302]</t>
         </is>
       </c>
       <c r="E32" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C302]</t>
         </is>
       </c>
       <c r="F32" s="8" t="inlineStr">
@@ -2246,12 +2246,12 @@
       </c>
       <c r="D33" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C303], Wed 09:00-10:30 [C303]</t>
         </is>
       </c>
       <c r="E33" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C303]</t>
         </is>
       </c>
       <c r="F33" s="8" t="inlineStr">
@@ -2279,12 +2279,12 @@
       </c>
       <c r="D34" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C304], Wed 09:00-10:30 [C304]</t>
         </is>
       </c>
       <c r="E34" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C304]</t>
         </is>
       </c>
       <c r="F34" s="8" t="inlineStr">
@@ -2406,7 +2406,7 @@
       </c>
       <c r="C3" s="10" t="inlineStr">
         <is>
-          <t>MA161 [C003]</t>
+          <t>MA161 [C004]</t>
         </is>
       </c>
       <c r="D3" s="9" t="inlineStr">
@@ -2434,17 +2434,17 @@
       </c>
       <c r="B4" s="10" t="inlineStr">
         <is>
-          <t>MA161 [C003]</t>
+          <t>MA161 [C004]</t>
         </is>
       </c>
       <c r="C4" s="13" t="inlineStr">
         <is>
-          <t>DS161 [C003]</t>
+          <t>DS161 [C004]</t>
         </is>
       </c>
       <c r="D4" s="14" t="inlineStr">
         <is>
-          <t>EC161 [C003]</t>
+          <t>EC161 [C004]</t>
         </is>
       </c>
       <c r="E4" s="12" t="inlineStr">
@@ -2500,22 +2500,22 @@
       </c>
       <c r="B6" s="13" t="inlineStr">
         <is>
-          <t>DS161 [C003]</t>
+          <t>DS161 [C004]</t>
         </is>
       </c>
       <c r="C6" s="16" t="inlineStr">
         <is>
-          <t>MA162 [C003]</t>
+          <t>MA162 [C004]</t>
         </is>
       </c>
       <c r="D6" s="14" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L105]</t>
+          <t>EC161 (Lab) [L206]</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [L207]</t>
+          <t>CS161 (Lab) [L107]</t>
         </is>
       </c>
       <c r="F6" s="8" t="inlineStr">
@@ -2543,12 +2543,12 @@
       </c>
       <c r="D7" s="14" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L105]</t>
+          <t>EC161 (Lab) [L206]</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [L207]</t>
+          <t>CS161 (Lab) [L107]</t>
         </is>
       </c>
       <c r="F7" s="9" t="inlineStr">
@@ -2566,12 +2566,12 @@
       </c>
       <c r="B8" s="16" t="inlineStr">
         <is>
-          <t>MA162 [C003]</t>
+          <t>MA162 [C004]</t>
         </is>
       </c>
       <c r="C8" s="14" t="inlineStr">
         <is>
-          <t>EC161 [C003]</t>
+          <t>EC161 [C004]</t>
         </is>
       </c>
       <c r="D8" s="11" t="inlineStr">
@@ -3038,7 +3038,7 @@
       </c>
       <c r="E25" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C101]</t>
         </is>
       </c>
       <c r="F25" s="8" t="inlineStr">
@@ -3066,12 +3066,12 @@
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C102], Wed 09:00-10:30 [C102]</t>
         </is>
       </c>
       <c r="E26" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C102]</t>
         </is>
       </c>
       <c r="F26" s="8" t="inlineStr">
@@ -3099,12 +3099,12 @@
       </c>
       <c r="D27" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C104], Wed 09:00-10:30 [C104]</t>
         </is>
       </c>
       <c r="E27" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C104]</t>
         </is>
       </c>
       <c r="F27" s="8" t="inlineStr">
@@ -3132,12 +3132,12 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C202], Wed 09:00-10:30 [C202]</t>
         </is>
       </c>
       <c r="E28" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C202]</t>
         </is>
       </c>
       <c r="F28" s="8" t="inlineStr">
@@ -3165,12 +3165,12 @@
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C203], Wed 09:00-10:30 [C203]</t>
         </is>
       </c>
       <c r="E29" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C203]</t>
         </is>
       </c>
       <c r="F29" s="8" t="inlineStr">
@@ -3198,12 +3198,12 @@
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C204], Wed 09:00-10:30 [C204]</t>
         </is>
       </c>
       <c r="E30" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C204]</t>
         </is>
       </c>
       <c r="F30" s="8" t="inlineStr">
@@ -3231,12 +3231,12 @@
       </c>
       <c r="D31" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C205], Wed 09:00-10:30 [C205]</t>
         </is>
       </c>
       <c r="E31" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C205]</t>
         </is>
       </c>
       <c r="F31" s="8" t="inlineStr">
@@ -3264,12 +3264,12 @@
       </c>
       <c r="D32" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C302], Wed 09:00-10:30 [C302]</t>
         </is>
       </c>
       <c r="E32" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C302]</t>
         </is>
       </c>
       <c r="F32" s="8" t="inlineStr">
@@ -3297,12 +3297,12 @@
       </c>
       <c r="D33" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C303], Wed 09:00-10:30 [C303]</t>
         </is>
       </c>
       <c r="E33" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C303]</t>
         </is>
       </c>
       <c r="F33" s="8" t="inlineStr">
@@ -3330,12 +3330,12 @@
       </c>
       <c r="D34" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C304], Wed 09:00-10:30 [C304]</t>
         </is>
       </c>
       <c r="E34" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C304]</t>
         </is>
       </c>
       <c r="F34" s="8" t="inlineStr">
@@ -3495,7 +3495,7 @@
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>MA161 [C003]</t>
+          <t>MA161 [C004]</t>
         </is>
       </c>
       <c r="E4" s="8" t="inlineStr">
@@ -3556,7 +3556,7 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>MA161 [C003]</t>
+          <t>MA161 [C004]</t>
         </is>
       </c>
       <c r="D6" s="13" t="inlineStr">
@@ -3622,7 +3622,7 @@
       </c>
       <c r="C8" s="13" t="inlineStr">
         <is>
-          <t>DS161 [C003]</t>
+          <t>DS161 [C004]</t>
         </is>
       </c>
       <c r="D8" s="8" t="inlineStr">
@@ -4089,7 +4089,7 @@
       </c>
       <c r="E25" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C101]</t>
         </is>
       </c>
       <c r="F25" s="8" t="inlineStr">
@@ -4117,12 +4117,12 @@
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C102], Wed 09:00-10:30 [C102]</t>
         </is>
       </c>
       <c r="E26" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C102]</t>
         </is>
       </c>
       <c r="F26" s="8" t="inlineStr">
@@ -4150,12 +4150,12 @@
       </c>
       <c r="D27" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C104], Wed 09:00-10:30 [C104]</t>
         </is>
       </c>
       <c r="E27" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C104]</t>
         </is>
       </c>
       <c r="F27" s="8" t="inlineStr">
@@ -4183,12 +4183,12 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C202], Wed 09:00-10:30 [C202]</t>
         </is>
       </c>
       <c r="E28" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C202]</t>
         </is>
       </c>
       <c r="F28" s="8" t="inlineStr">
@@ -4216,12 +4216,12 @@
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C203], Wed 09:00-10:30 [C203]</t>
         </is>
       </c>
       <c r="E29" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C203]</t>
         </is>
       </c>
       <c r="F29" s="8" t="inlineStr">
@@ -4249,12 +4249,12 @@
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C204], Wed 09:00-10:30 [C204]</t>
         </is>
       </c>
       <c r="E30" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C204]</t>
         </is>
       </c>
       <c r="F30" s="8" t="inlineStr">
@@ -4282,12 +4282,12 @@
       </c>
       <c r="D31" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C205], Wed 09:00-10:30 [C205]</t>
         </is>
       </c>
       <c r="E31" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C205]</t>
         </is>
       </c>
       <c r="F31" s="8" t="inlineStr">
@@ -4315,12 +4315,12 @@
       </c>
       <c r="D32" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C302], Wed 09:00-10:30 [C302]</t>
         </is>
       </c>
       <c r="E32" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C302]</t>
         </is>
       </c>
       <c r="F32" s="8" t="inlineStr">
@@ -4348,12 +4348,12 @@
       </c>
       <c r="D33" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C303], Wed 09:00-10:30 [C303]</t>
         </is>
       </c>
       <c r="E33" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C303]</t>
         </is>
       </c>
       <c r="F33" s="8" t="inlineStr">
@@ -4381,12 +4381,12 @@
       </c>
       <c r="D34" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C304], Wed 09:00-10:30 [C304]</t>
         </is>
       </c>
       <c r="E34" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C304]</t>
         </is>
       </c>
       <c r="F34" s="8" t="inlineStr">
@@ -4536,7 +4536,7 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>CS161 [C102]</t>
+          <t>CS161 [C101]</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
@@ -4546,7 +4546,7 @@
       </c>
       <c r="D4" s="10" t="inlineStr">
         <is>
-          <t>MA161 [C003]</t>
+          <t>MA161 [C004]</t>
         </is>
       </c>
       <c r="E4" s="8" t="inlineStr">
@@ -4607,12 +4607,12 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>MA161 [C003]</t>
+          <t>MA161 [C004]</t>
         </is>
       </c>
       <c r="D6" s="13" t="inlineStr">
         <is>
-          <t>DS161 [C003]</t>
+          <t>DS161 [C004]</t>
         </is>
       </c>
       <c r="E6" s="8" t="inlineStr">
@@ -4668,12 +4668,12 @@
       </c>
       <c r="B8" s="12" t="inlineStr">
         <is>
-          <t>HS161 [C102]</t>
+          <t>HS161 [C101]</t>
         </is>
       </c>
       <c r="C8" s="13" t="inlineStr">
         <is>
-          <t>DS161 [C003]</t>
+          <t>DS161 [C004]</t>
         </is>
       </c>
       <c r="D8" s="8" t="inlineStr">
@@ -5140,7 +5140,7 @@
       </c>
       <c r="E25" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C101]</t>
         </is>
       </c>
       <c r="F25" s="8" t="inlineStr">
@@ -5168,12 +5168,12 @@
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C102], Wed 09:00-10:30 [C102]</t>
         </is>
       </c>
       <c r="E26" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C102]</t>
         </is>
       </c>
       <c r="F26" s="8" t="inlineStr">
@@ -5201,12 +5201,12 @@
       </c>
       <c r="D27" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C104], Wed 09:00-10:30 [C104]</t>
         </is>
       </c>
       <c r="E27" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C104]</t>
         </is>
       </c>
       <c r="F27" s="8" t="inlineStr">
@@ -5234,12 +5234,12 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C202], Wed 09:00-10:30 [C202]</t>
         </is>
       </c>
       <c r="E28" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C202]</t>
         </is>
       </c>
       <c r="F28" s="8" t="inlineStr">
@@ -5267,12 +5267,12 @@
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C203], Wed 09:00-10:30 [C203]</t>
         </is>
       </c>
       <c r="E29" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C203]</t>
         </is>
       </c>
       <c r="F29" s="8" t="inlineStr">
@@ -5300,12 +5300,12 @@
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C204], Wed 09:00-10:30 [C204]</t>
         </is>
       </c>
       <c r="E30" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C204]</t>
         </is>
       </c>
       <c r="F30" s="8" t="inlineStr">
@@ -5333,12 +5333,12 @@
       </c>
       <c r="D31" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C205], Wed 09:00-10:30 [C205]</t>
         </is>
       </c>
       <c r="E31" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C205]</t>
         </is>
       </c>
       <c r="F31" s="8" t="inlineStr">
@@ -5366,12 +5366,12 @@
       </c>
       <c r="D32" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C302], Wed 09:00-10:30 [C302]</t>
         </is>
       </c>
       <c r="E32" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C302]</t>
         </is>
       </c>
       <c r="F32" s="8" t="inlineStr">
@@ -5399,12 +5399,12 @@
       </c>
       <c r="D33" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C303], Wed 09:00-10:30 [C303]</t>
         </is>
       </c>
       <c r="E33" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C303]</t>
         </is>
       </c>
       <c r="F33" s="8" t="inlineStr">
@@ -5432,12 +5432,12 @@
       </c>
       <c r="D34" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C304], Wed 09:00-10:30 [C304]</t>
         </is>
       </c>
       <c r="E34" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C304]</t>
         </is>
       </c>
       <c r="F34" s="8" t="inlineStr">
@@ -5587,7 +5587,7 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>CS161 [C104]</t>
+          <t>CS161 [C102]</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
@@ -5597,7 +5597,7 @@
       </c>
       <c r="D4" s="16" t="inlineStr">
         <is>
-          <t>MA162 [C003]</t>
+          <t>MA162 [C004]</t>
         </is>
       </c>
       <c r="E4" s="8" t="inlineStr">
@@ -5658,12 +5658,12 @@
       </c>
       <c r="C6" s="16" t="inlineStr">
         <is>
-          <t>MA162 [C003]</t>
+          <t>MA162 [C004]</t>
         </is>
       </c>
       <c r="D6" s="14" t="inlineStr">
         <is>
-          <t>EC161 [C003]</t>
+          <t>EC161 [C004]</t>
         </is>
       </c>
       <c r="E6" s="8" t="inlineStr">
@@ -5719,17 +5719,17 @@
       </c>
       <c r="B8" s="12" t="inlineStr">
         <is>
-          <t>HS161 [C104]</t>
+          <t>HS161 [C102]</t>
         </is>
       </c>
       <c r="C8" s="14" t="inlineStr">
         <is>
-          <t>EC161 [C003]</t>
+          <t>EC161 [C004]</t>
         </is>
       </c>
       <c r="D8" s="14" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L206]</t>
+          <t>EC161 (Lab) [L105]</t>
         </is>
       </c>
       <c r="E8" s="8" t="inlineStr">
@@ -5762,7 +5762,7 @@
       </c>
       <c r="D9" s="14" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L206]</t>
+          <t>EC161 (Lab) [L105]</t>
         </is>
       </c>
       <c r="E9" s="8" t="inlineStr">
@@ -6191,7 +6191,7 @@
       </c>
       <c r="E25" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C101]</t>
         </is>
       </c>
       <c r="F25" s="8" t="inlineStr">
@@ -6219,12 +6219,12 @@
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C102], Wed 09:00-10:30 [C102]</t>
         </is>
       </c>
       <c r="E26" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C102]</t>
         </is>
       </c>
       <c r="F26" s="8" t="inlineStr">
@@ -6252,12 +6252,12 @@
       </c>
       <c r="D27" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C104], Wed 09:00-10:30 [C104]</t>
         </is>
       </c>
       <c r="E27" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C104]</t>
         </is>
       </c>
       <c r="F27" s="8" t="inlineStr">
@@ -6285,12 +6285,12 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C202], Wed 09:00-10:30 [C202]</t>
         </is>
       </c>
       <c r="E28" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C202]</t>
         </is>
       </c>
       <c r="F28" s="8" t="inlineStr">
@@ -6318,12 +6318,12 @@
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C203], Wed 09:00-10:30 [C203]</t>
         </is>
       </c>
       <c r="E29" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C203]</t>
         </is>
       </c>
       <c r="F29" s="8" t="inlineStr">
@@ -6351,12 +6351,12 @@
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C204], Wed 09:00-10:30 [C204]</t>
         </is>
       </c>
       <c r="E30" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C204]</t>
         </is>
       </c>
       <c r="F30" s="8" t="inlineStr">
@@ -6384,12 +6384,12 @@
       </c>
       <c r="D31" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C205], Wed 09:00-10:30 [C205]</t>
         </is>
       </c>
       <c r="E31" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C205]</t>
         </is>
       </c>
       <c r="F31" s="8" t="inlineStr">
@@ -6417,12 +6417,12 @@
       </c>
       <c r="D32" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C302], Wed 09:00-10:30 [C302]</t>
         </is>
       </c>
       <c r="E32" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C302]</t>
         </is>
       </c>
       <c r="F32" s="8" t="inlineStr">
@@ -6450,12 +6450,12 @@
       </c>
       <c r="D33" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C303], Wed 09:00-10:30 [C303]</t>
         </is>
       </c>
       <c r="E33" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C303]</t>
         </is>
       </c>
       <c r="F33" s="8" t="inlineStr">
@@ -6483,12 +6483,12 @@
       </c>
       <c r="D34" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C304], Wed 09:00-10:30 [C304]</t>
         </is>
       </c>
       <c r="E34" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C304]</t>
         </is>
       </c>
       <c r="F34" s="8" t="inlineStr">
@@ -6638,7 +6638,7 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>CS161 [C203]</t>
+          <t>CS161 [C104]</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
@@ -6648,7 +6648,7 @@
       </c>
       <c r="D4" s="16" t="inlineStr">
         <is>
-          <t>MA162 [C003]</t>
+          <t>MA162 [C004]</t>
         </is>
       </c>
       <c r="E4" s="8" t="inlineStr">
@@ -6709,12 +6709,12 @@
       </c>
       <c r="C6" s="16" t="inlineStr">
         <is>
-          <t>MA162 [C003]</t>
+          <t>MA162 [C004]</t>
         </is>
       </c>
       <c r="D6" s="14" t="inlineStr">
         <is>
-          <t>EC161 [C003]</t>
+          <t>EC161 [C004]</t>
         </is>
       </c>
       <c r="E6" s="8" t="inlineStr">
@@ -6770,17 +6770,17 @@
       </c>
       <c r="B8" s="12" t="inlineStr">
         <is>
-          <t>HS161 [C203]</t>
+          <t>HS161 [C104]</t>
         </is>
       </c>
       <c r="C8" s="14" t="inlineStr">
         <is>
-          <t>EC161 [C003]</t>
+          <t>EC161 [C004]</t>
         </is>
       </c>
       <c r="D8" s="14" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L105]</t>
+          <t>EC161 (Lab) [L206]</t>
         </is>
       </c>
       <c r="E8" s="8" t="inlineStr">
@@ -6813,7 +6813,7 @@
       </c>
       <c r="D9" s="14" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L105]</t>
+          <t>EC161 (Lab) [L206]</t>
         </is>
       </c>
       <c r="E9" s="8" t="inlineStr">
@@ -7242,7 +7242,7 @@
       </c>
       <c r="E25" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C101]</t>
         </is>
       </c>
       <c r="F25" s="8" t="inlineStr">
@@ -7270,12 +7270,12 @@
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C102], Wed 09:00-10:30 [C102]</t>
         </is>
       </c>
       <c r="E26" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C102]</t>
         </is>
       </c>
       <c r="F26" s="8" t="inlineStr">
@@ -7303,12 +7303,12 @@
       </c>
       <c r="D27" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C104], Wed 09:00-10:30 [C104]</t>
         </is>
       </c>
       <c r="E27" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C104]</t>
         </is>
       </c>
       <c r="F27" s="8" t="inlineStr">
@@ -7336,12 +7336,12 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C202], Wed 09:00-10:30 [C202]</t>
         </is>
       </c>
       <c r="E28" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C202]</t>
         </is>
       </c>
       <c r="F28" s="8" t="inlineStr">
@@ -7369,12 +7369,12 @@
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C203], Wed 09:00-10:30 [C203]</t>
         </is>
       </c>
       <c r="E29" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C203]</t>
         </is>
       </c>
       <c r="F29" s="8" t="inlineStr">
@@ -7402,12 +7402,12 @@
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C204], Wed 09:00-10:30 [C204]</t>
         </is>
       </c>
       <c r="E30" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C204]</t>
         </is>
       </c>
       <c r="F30" s="8" t="inlineStr">
@@ -7435,12 +7435,12 @@
       </c>
       <c r="D31" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C205], Wed 09:00-10:30 [C205]</t>
         </is>
       </c>
       <c r="E31" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C205]</t>
         </is>
       </c>
       <c r="F31" s="8" t="inlineStr">
@@ -7468,12 +7468,12 @@
       </c>
       <c r="D32" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C302], Wed 09:00-10:30 [C302]</t>
         </is>
       </c>
       <c r="E32" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C302]</t>
         </is>
       </c>
       <c r="F32" s="8" t="inlineStr">
@@ -7501,12 +7501,12 @@
       </c>
       <c r="D33" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C303], Wed 09:00-10:30 [C303]</t>
         </is>
       </c>
       <c r="E33" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C303]</t>
         </is>
       </c>
       <c r="F33" s="8" t="inlineStr">
@@ -7534,12 +7534,12 @@
       </c>
       <c r="D34" s="8" t="inlineStr">
         <is>
-          <t>Mon 09:00-10:30 [C101], Wed 09:00-10:30 [C101]</t>
+          <t>Mon 09:00-10:30 [C304], Wed 09:00-10:30 [C304]</t>
         </is>
       </c>
       <c r="E34" s="8" t="inlineStr">
         <is>
-          <t>Fri 14:30-15:30</t>
+          <t>Fri 14:30-15:30 [C304]</t>
         </is>
       </c>
       <c r="F34" s="8" t="inlineStr">

</xml_diff>

<commit_message>
Added Faculty details to excel timetables
</commit_message>
<xml_diff>
--- a/backend/output_timetables/sem1_CSE_timetable.xlsx
+++ b/backend/output_timetables/sem1_CSE_timetable.xlsx
@@ -772,7 +772,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -784,7 +784,8 @@
     <col width="40" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
     <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="35" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="35" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -824,6 +825,11 @@
       </c>
       <c r="E4" s="4" t="inlineStr">
         <is>
+          <t>Faculty</t>
+        </is>
+      </c>
+      <c r="F4" s="4" t="inlineStr">
+        <is>
           <t>Display Format</t>
         </is>
       </c>
@@ -851,6 +857,11 @@
       </c>
       <c r="E5" s="5" t="inlineStr">
         <is>
+          <t>Sunil P V, Sunil C K, Animesh Roy</t>
+        </is>
+      </c>
+      <c r="F5" s="5" t="inlineStr">
+        <is>
           <t>CS161 (3-0-2-0-4 | Full Sem)</t>
         </is>
       </c>
@@ -878,6 +889,11 @@
       </c>
       <c r="E6" s="5" t="inlineStr">
         <is>
+          <t>Abdul Wahid</t>
+        </is>
+      </c>
+      <c r="F6" s="5" t="inlineStr">
+        <is>
           <t>DS161 (2-0-0-0-2 | Pre-Mid Only)</t>
         </is>
       </c>
@@ -905,6 +921,11 @@
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
+          <t>Prakash Pawar</t>
+        </is>
+      </c>
+      <c r="F7" s="5" t="inlineStr">
+        <is>
           <t>EC161 (3-0-2-0-2 | Post-Mid Only)</t>
         </is>
       </c>
@@ -932,6 +953,11 @@
       </c>
       <c r="E8" s="5" t="inlineStr">
         <is>
+          <t>Rajesh N S</t>
+        </is>
+      </c>
+      <c r="F8" s="5" t="inlineStr">
+        <is>
           <t>HS161 (3-0-0-0-3 | Full Sem)</t>
         </is>
       </c>
@@ -959,6 +985,11 @@
       </c>
       <c r="E9" s="5" t="inlineStr">
         <is>
+          <t>Ramesh Athe</t>
+        </is>
+      </c>
+      <c r="F9" s="5" t="inlineStr">
+        <is>
           <t>MA161 (2-0-0-0-2 | Pre-Mid Only)</t>
         </is>
       </c>
@@ -986,6 +1017,11 @@
       </c>
       <c r="E10" s="5" t="inlineStr">
         <is>
+          <t>Chinmayananda</t>
+        </is>
+      </c>
+      <c r="F10" s="5" t="inlineStr">
+        <is>
           <t>MA162 (2-0-0-0-2 | Post-Mid Only)</t>
         </is>
       </c>
@@ -1020,6 +1056,11 @@
       </c>
       <c r="E13" s="4" t="inlineStr">
         <is>
+          <t>Faculty</t>
+        </is>
+      </c>
+      <c r="F13" s="4" t="inlineStr">
+        <is>
           <t>Display Format</t>
         </is>
       </c>
@@ -1047,6 +1088,11 @@
       </c>
       <c r="E14" s="5" t="inlineStr">
         <is>
+          <t>Mallikarjun Kande</t>
+        </is>
+      </c>
+      <c r="F14" s="5" t="inlineStr">
+        <is>
           <t>CS101 (2-0-0-0-2)</t>
         </is>
       </c>
@@ -1074,6 +1120,11 @@
       </c>
       <c r="E15" s="5" t="inlineStr">
         <is>
+          <t>Girish Revadigar</t>
+        </is>
+      </c>
+      <c r="F15" s="5" t="inlineStr">
+        <is>
           <t>CS151 (2-0-0-0-2)</t>
         </is>
       </c>
@@ -1101,6 +1152,11 @@
       </c>
       <c r="E16" s="5" t="inlineStr">
         <is>
+          <t>Sandesh Phalke</t>
+        </is>
+      </c>
+      <c r="F16" s="5" t="inlineStr">
+        <is>
           <t>DE101 (2-0-0-0-2)</t>
         </is>
       </c>
@@ -1128,6 +1184,11 @@
       </c>
       <c r="E17" s="5" t="inlineStr">
         <is>
+          <t>Vivekraj</t>
+        </is>
+      </c>
+      <c r="F17" s="5" t="inlineStr">
+        <is>
           <t>DS151 (2-0-0-0-2)</t>
         </is>
       </c>
@@ -1155,6 +1216,11 @@
       </c>
       <c r="E18" s="5" t="inlineStr">
         <is>
+          <t>Anand B</t>
+        </is>
+      </c>
+      <c r="F18" s="5" t="inlineStr">
+        <is>
           <t>HS102 (2-0-0-0-2)</t>
         </is>
       </c>
@@ -1182,6 +1248,11 @@
       </c>
       <c r="E19" s="5" t="inlineStr">
         <is>
+          <t>Rajesh N S</t>
+        </is>
+      </c>
+      <c r="F19" s="5" t="inlineStr">
+        <is>
           <t>HS103 (2-0-0-0-2)</t>
         </is>
       </c>
@@ -1209,6 +1280,11 @@
       </c>
       <c r="E20" s="5" t="inlineStr">
         <is>
+          <t>Anushree Kini</t>
+        </is>
+      </c>
+      <c r="F20" s="5" t="inlineStr">
+        <is>
           <t>HS152 (3-0-0-0-3)</t>
         </is>
       </c>
@@ -1236,6 +1312,11 @@
       </c>
       <c r="E21" s="5" t="inlineStr">
         <is>
+          <t>Rajesh N S</t>
+        </is>
+      </c>
+      <c r="F21" s="5" t="inlineStr">
+        <is>
           <t>HS156 (1-0-0-0-1)</t>
         </is>
       </c>
@@ -1263,6 +1344,11 @@
       </c>
       <c r="E22" s="5" t="inlineStr">
         <is>
+          <t>Chandrika Kamat</t>
+        </is>
+      </c>
+      <c r="F22" s="5" t="inlineStr">
+        <is>
           <t>HS157 (1-0-0-0-1)</t>
         </is>
       </c>
@@ -1290,15 +1376,20 @@
       </c>
       <c r="E23" s="5" t="inlineStr">
         <is>
+          <t>Ravishankar, Vivekraj</t>
+        </is>
+      </c>
+      <c r="F23" s="5" t="inlineStr">
+        <is>
           <t>PH151 (2-0-0-0-2)</t>
         </is>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A12:F12"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1475,10 +1566,10 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>151.5</v>
+        <v>150</v>
       </c>
       <c r="E5" t="n">
-        <v>30.3</v>
+        <v>30</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -1543,10 +1634,10 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1.5</v>
+        <v>6</v>
       </c>
       <c r="E7" t="n">
-        <v>0.3</v>
+        <v>1.2</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -1611,10 +1702,10 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -1713,10 +1804,10 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -1849,10 +1940,10 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -1883,10 +1974,10 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
@@ -1951,10 +2042,10 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -1985,10 +2076,10 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
@@ -2087,10 +2178,10 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
@@ -2121,10 +2212,10 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F24" t="n">
         <v>0</v>
@@ -2155,10 +2246,10 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
@@ -2189,10 +2280,10 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="F26" t="n">
         <v>0</v>
@@ -2475,10 +2566,10 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F35" t="n">
         <v>0</v>
@@ -2509,10 +2600,10 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="F36" t="n">
         <v>0</v>
@@ -2543,10 +2634,10 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="F37" t="n">
         <v>0</v>
@@ -2702,7 +2793,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J2" t="b">
@@ -2716,7 +2807,7 @@
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
-          <t>C305</t>
+          <t>C102</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -2788,7 +2879,7 @@
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr">
         <is>
-          <t>L107</t>
+          <t>L207</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -2860,7 +2951,7 @@
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr">
         <is>
-          <t>L208</t>
+          <t>L207</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -2918,7 +3009,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J5" t="b">
@@ -2932,7 +3023,7 @@
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr">
         <is>
-          <t>C304</t>
+          <t>C102</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -2985,12 +3076,12 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J6" t="b">
@@ -3004,7 +3095,7 @@
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr">
         <is>
-          <t>L406</t>
+          <t>C302</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -3489,12 +3580,12 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J13" t="b">
@@ -3508,7 +3599,7 @@
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr">
         <is>
-          <t>L406</t>
+          <t>C302</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
@@ -3566,7 +3657,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J14" t="b">
@@ -3580,7 +3671,7 @@
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr">
         <is>
-          <t>C305</t>
+          <t>C102</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
@@ -3849,12 +3940,12 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J18" t="b">
@@ -3868,7 +3959,7 @@
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr">
         <is>
-          <t>L406</t>
+          <t>C302</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
@@ -4353,12 +4444,12 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J25" t="b">
@@ -4372,7 +4463,7 @@
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="inlineStr">
         <is>
-          <t>L406</t>
+          <t>C302</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
@@ -4588,7 +4679,7 @@
       <c r="L28" t="inlineStr"/>
       <c r="M28" t="inlineStr">
         <is>
-          <t>L206</t>
+          <t>L105</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
@@ -4660,7 +4751,7 @@
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="inlineStr">
         <is>
-          <t>L206</t>
+          <t>L105</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
@@ -4713,12 +4804,12 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J30" t="b">
@@ -4732,7 +4823,7 @@
       <c r="L30" t="inlineStr"/>
       <c r="M30" t="inlineStr">
         <is>
-          <t>L406</t>
+          <t>C302</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
@@ -5217,12 +5308,12 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J37" t="b">
@@ -5236,7 +5327,7 @@
       <c r="L37" t="inlineStr"/>
       <c r="M37" t="inlineStr">
         <is>
-          <t>L406</t>
+          <t>C302</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
@@ -5289,12 +5380,12 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J38" t="b">
@@ -5308,7 +5399,7 @@
       <c r="L38" t="inlineStr"/>
       <c r="M38" t="inlineStr">
         <is>
-          <t>L406</t>
+          <t>C302</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
@@ -5793,12 +5884,12 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J45" t="b">
@@ -5812,7 +5903,7 @@
       <c r="L45" t="inlineStr"/>
       <c r="M45" t="inlineStr">
         <is>
-          <t>L406</t>
+          <t>C302</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
@@ -5865,12 +5956,12 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J46" t="b">
@@ -5884,7 +5975,7 @@
       <c r="L46" t="inlineStr"/>
       <c r="M46" t="inlineStr">
         <is>
-          <t>L406</t>
+          <t>C302</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
@@ -6369,12 +6460,12 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J53" t="b">
@@ -6388,7 +6479,7 @@
       <c r="L53" t="inlineStr"/>
       <c r="M53" t="inlineStr">
         <is>
-          <t>L406</t>
+          <t>C302</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
@@ -6446,7 +6537,7 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J54" t="b">
@@ -6464,7 +6555,7 @@
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>C203</t>
+          <t>C101</t>
         </is>
       </c>
       <c r="N54" t="inlineStr">
@@ -6522,7 +6613,7 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J55" t="b">
@@ -6540,7 +6631,7 @@
       </c>
       <c r="M55" t="inlineStr">
         <is>
-          <t>C204</t>
+          <t>C102</t>
         </is>
       </c>
       <c r="N55" t="inlineStr">
@@ -6598,7 +6689,7 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J56" t="b">
@@ -6616,7 +6707,7 @@
       </c>
       <c r="M56" t="inlineStr">
         <is>
-          <t>C205</t>
+          <t>C104</t>
         </is>
       </c>
       <c r="N56" t="inlineStr">
@@ -6692,7 +6783,7 @@
       </c>
       <c r="M57" t="inlineStr">
         <is>
-          <t>C302</t>
+          <t>C202</t>
         </is>
       </c>
       <c r="N57" t="inlineStr">
@@ -6768,7 +6859,7 @@
       </c>
       <c r="M58" t="inlineStr">
         <is>
-          <t>C303</t>
+          <t>C203</t>
         </is>
       </c>
       <c r="N58" t="inlineStr">
@@ -6844,7 +6935,7 @@
       </c>
       <c r="M59" t="inlineStr">
         <is>
-          <t>C304</t>
+          <t>C204</t>
         </is>
       </c>
       <c r="N59" t="inlineStr">
@@ -6920,7 +7011,7 @@
       </c>
       <c r="M60" t="inlineStr">
         <is>
-          <t>C305</t>
+          <t>C205</t>
         </is>
       </c>
       <c r="N60" t="inlineStr">
@@ -6968,15 +7059,19 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="I61" t="inlineStr"/>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
       <c r="J61" t="b">
         <v>0</v>
       </c>
@@ -6992,7 +7087,7 @@
       </c>
       <c r="M61" t="inlineStr">
         <is>
-          <t>C001</t>
+          <t>C302</t>
         </is>
       </c>
       <c r="N61" t="inlineStr">
@@ -7040,17 +7135,17 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>Projector</t>
+          <t>TV</t>
         </is>
       </c>
       <c r="J62" t="b">
@@ -7068,7 +7163,7 @@
       </c>
       <c r="M62" t="inlineStr">
         <is>
-          <t>C002</t>
+          <t>C303</t>
         </is>
       </c>
       <c r="N62" t="inlineStr">
@@ -7116,17 +7211,17 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>Projector</t>
+          <t>TV</t>
         </is>
       </c>
       <c r="J63" t="b">
@@ -7144,7 +7239,7 @@
       </c>
       <c r="M63" t="inlineStr">
         <is>
-          <t>C003</t>
+          <t>C304</t>
         </is>
       </c>
       <c r="N63" t="inlineStr">
@@ -8112,7 +8207,7 @@
       <c r="L76" t="inlineStr"/>
       <c r="M76" t="inlineStr">
         <is>
-          <t>L206</t>
+          <t>L105</t>
         </is>
       </c>
       <c r="N76" t="inlineStr">
@@ -8642,7 +8737,7 @@
       </c>
       <c r="I84" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J84" t="b">
@@ -8660,7 +8755,7 @@
       </c>
       <c r="M84" t="inlineStr">
         <is>
-          <t>C203</t>
+          <t>C101</t>
         </is>
       </c>
       <c r="N84" t="inlineStr">
@@ -8718,7 +8813,7 @@
       </c>
       <c r="I85" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J85" t="b">
@@ -8736,7 +8831,7 @@
       </c>
       <c r="M85" t="inlineStr">
         <is>
-          <t>C204</t>
+          <t>C102</t>
         </is>
       </c>
       <c r="N85" t="inlineStr">
@@ -8794,7 +8889,7 @@
       </c>
       <c r="I86" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J86" t="b">
@@ -8812,7 +8907,7 @@
       </c>
       <c r="M86" t="inlineStr">
         <is>
-          <t>C205</t>
+          <t>C104</t>
         </is>
       </c>
       <c r="N86" t="inlineStr">
@@ -8888,7 +8983,7 @@
       </c>
       <c r="M87" t="inlineStr">
         <is>
-          <t>C302</t>
+          <t>C202</t>
         </is>
       </c>
       <c r="N87" t="inlineStr">
@@ -8964,7 +9059,7 @@
       </c>
       <c r="M88" t="inlineStr">
         <is>
-          <t>C303</t>
+          <t>C203</t>
         </is>
       </c>
       <c r="N88" t="inlineStr">
@@ -9040,7 +9135,7 @@
       </c>
       <c r="M89" t="inlineStr">
         <is>
-          <t>C304</t>
+          <t>C204</t>
         </is>
       </c>
       <c r="N89" t="inlineStr">
@@ -9116,7 +9211,7 @@
       </c>
       <c r="M90" t="inlineStr">
         <is>
-          <t>C305</t>
+          <t>C205</t>
         </is>
       </c>
       <c r="N90" t="inlineStr">
@@ -9164,15 +9259,19 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="I91" t="inlineStr"/>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
       <c r="J91" t="b">
         <v>0</v>
       </c>
@@ -9188,7 +9287,7 @@
       </c>
       <c r="M91" t="inlineStr">
         <is>
-          <t>C001</t>
+          <t>C302</t>
         </is>
       </c>
       <c r="N91" t="inlineStr">
@@ -9236,17 +9335,17 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I92" t="inlineStr">
         <is>
-          <t>Projector</t>
+          <t>TV</t>
         </is>
       </c>
       <c r="J92" t="b">
@@ -9264,7 +9363,7 @@
       </c>
       <c r="M92" t="inlineStr">
         <is>
-          <t>C002</t>
+          <t>C303</t>
         </is>
       </c>
       <c r="N92" t="inlineStr">
@@ -9312,17 +9411,17 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I93" t="inlineStr">
         <is>
-          <t>Projector</t>
+          <t>TV</t>
         </is>
       </c>
       <c r="J93" t="b">
@@ -9340,7 +9439,7 @@
       </c>
       <c r="M93" t="inlineStr">
         <is>
-          <t>C003</t>
+          <t>C304</t>
         </is>
       </c>
       <c r="N93" t="inlineStr">
@@ -9466,7 +9565,7 @@
       </c>
       <c r="I95" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J95" t="b">
@@ -9480,7 +9579,7 @@
       <c r="L95" t="inlineStr"/>
       <c r="M95" t="inlineStr">
         <is>
-          <t>C204</t>
+          <t>C104</t>
         </is>
       </c>
       <c r="N95" t="inlineStr">
@@ -9552,7 +9651,7 @@
       <c r="L96" t="inlineStr"/>
       <c r="M96" t="inlineStr">
         <is>
-          <t>L107</t>
+          <t>L207</t>
         </is>
       </c>
       <c r="N96" t="inlineStr">
@@ -9600,21 +9699,21 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>Software Lab</t>
         </is>
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>40</t>
         </is>
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Computers</t>
         </is>
       </c>
       <c r="J97" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K97" t="inlineStr">
         <is>
@@ -9624,7 +9723,7 @@
       <c r="L97" t="inlineStr"/>
       <c r="M97" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>L207</t>
         </is>
       </c>
       <c r="N97" t="inlineStr">
@@ -9638,7 +9737,7 @@
         </is>
       </c>
       <c r="P97" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98">
@@ -9682,7 +9781,7 @@
       </c>
       <c r="I98" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J98" t="b">
@@ -9696,7 +9795,7 @@
       <c r="L98" t="inlineStr"/>
       <c r="M98" t="inlineStr">
         <is>
-          <t>C305</t>
+          <t>C104</t>
         </is>
       </c>
       <c r="N98" t="inlineStr">
@@ -9749,7 +9848,7 @@
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I99" t="inlineStr">
@@ -9768,7 +9867,7 @@
       <c r="L99" t="inlineStr"/>
       <c r="M99" t="inlineStr">
         <is>
-          <t>L408</t>
+          <t>C303</t>
         </is>
       </c>
       <c r="N99" t="inlineStr">
@@ -10253,7 +10352,7 @@
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I106" t="inlineStr">
@@ -10272,7 +10371,7 @@
       <c r="L106" t="inlineStr"/>
       <c r="M106" t="inlineStr">
         <is>
-          <t>L408</t>
+          <t>C303</t>
         </is>
       </c>
       <c r="N106" t="inlineStr">
@@ -10330,7 +10429,7 @@
       </c>
       <c r="I107" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J107" t="b">
@@ -10344,7 +10443,7 @@
       <c r="L107" t="inlineStr"/>
       <c r="M107" t="inlineStr">
         <is>
-          <t>C204</t>
+          <t>C104</t>
         </is>
       </c>
       <c r="N107" t="inlineStr">
@@ -10402,7 +10501,7 @@
       </c>
       <c r="I108" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J108" t="b">
@@ -10416,7 +10515,7 @@
       <c r="L108" t="inlineStr"/>
       <c r="M108" t="inlineStr">
         <is>
-          <t>C205</t>
+          <t>C104</t>
         </is>
       </c>
       <c r="N108" t="inlineStr">
@@ -10613,7 +10712,7 @@
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I111" t="inlineStr">
@@ -10632,7 +10731,7 @@
       <c r="L111" t="inlineStr"/>
       <c r="M111" t="inlineStr">
         <is>
-          <t>L408</t>
+          <t>C303</t>
         </is>
       </c>
       <c r="N111" t="inlineStr">
@@ -11117,7 +11216,7 @@
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I118" t="inlineStr">
@@ -11136,7 +11235,7 @@
       <c r="L118" t="inlineStr"/>
       <c r="M118" t="inlineStr">
         <is>
-          <t>L408</t>
+          <t>C303</t>
         </is>
       </c>
       <c r="N118" t="inlineStr">
@@ -11352,7 +11451,7 @@
       <c r="L121" t="inlineStr"/>
       <c r="M121" t="inlineStr">
         <is>
-          <t>L105</t>
+          <t>L206</t>
         </is>
       </c>
       <c r="N121" t="inlineStr">
@@ -11424,7 +11523,7 @@
       <c r="L122" t="inlineStr"/>
       <c r="M122" t="inlineStr">
         <is>
-          <t>L105</t>
+          <t>L206</t>
         </is>
       </c>
       <c r="N122" t="inlineStr">
@@ -11477,7 +11576,7 @@
       </c>
       <c r="H123" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I123" t="inlineStr">
@@ -11496,7 +11595,7 @@
       <c r="L123" t="inlineStr"/>
       <c r="M123" t="inlineStr">
         <is>
-          <t>L408</t>
+          <t>C303</t>
         </is>
       </c>
       <c r="N123" t="inlineStr">
@@ -11981,7 +12080,7 @@
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I130" t="inlineStr">
@@ -12000,7 +12099,7 @@
       <c r="L130" t="inlineStr"/>
       <c r="M130" t="inlineStr">
         <is>
-          <t>L408</t>
+          <t>C303</t>
         </is>
       </c>
       <c r="N130" t="inlineStr">
@@ -12053,7 +12152,7 @@
       </c>
       <c r="H131" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I131" t="inlineStr">
@@ -12072,7 +12171,7 @@
       <c r="L131" t="inlineStr"/>
       <c r="M131" t="inlineStr">
         <is>
-          <t>L407</t>
+          <t>C303</t>
         </is>
       </c>
       <c r="N131" t="inlineStr">
@@ -12557,7 +12656,7 @@
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I138" t="inlineStr">
@@ -12576,7 +12675,7 @@
       <c r="L138" t="inlineStr"/>
       <c r="M138" t="inlineStr">
         <is>
-          <t>L408</t>
+          <t>C303</t>
         </is>
       </c>
       <c r="N138" t="inlineStr">
@@ -12629,7 +12728,7 @@
       </c>
       <c r="H139" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I139" t="inlineStr">
@@ -12648,7 +12747,7 @@
       <c r="L139" t="inlineStr"/>
       <c r="M139" t="inlineStr">
         <is>
-          <t>L407</t>
+          <t>C303</t>
         </is>
       </c>
       <c r="N139" t="inlineStr">
@@ -13133,7 +13232,7 @@
       </c>
       <c r="H146" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I146" t="inlineStr">
@@ -13152,7 +13251,7 @@
       <c r="L146" t="inlineStr"/>
       <c r="M146" t="inlineStr">
         <is>
-          <t>L408</t>
+          <t>C303</t>
         </is>
       </c>
       <c r="N146" t="inlineStr">
@@ -13210,7 +13309,7 @@
       </c>
       <c r="I147" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J147" t="b">
@@ -13228,7 +13327,7 @@
       </c>
       <c r="M147" t="inlineStr">
         <is>
-          <t>C203</t>
+          <t>C101</t>
         </is>
       </c>
       <c r="N147" t="inlineStr">
@@ -13286,7 +13385,7 @@
       </c>
       <c r="I148" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J148" t="b">
@@ -13304,7 +13403,7 @@
       </c>
       <c r="M148" t="inlineStr">
         <is>
-          <t>C204</t>
+          <t>C102</t>
         </is>
       </c>
       <c r="N148" t="inlineStr">
@@ -13362,7 +13461,7 @@
       </c>
       <c r="I149" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J149" t="b">
@@ -13380,7 +13479,7 @@
       </c>
       <c r="M149" t="inlineStr">
         <is>
-          <t>C205</t>
+          <t>C104</t>
         </is>
       </c>
       <c r="N149" t="inlineStr">
@@ -13456,7 +13555,7 @@
       </c>
       <c r="M150" t="inlineStr">
         <is>
-          <t>C302</t>
+          <t>C202</t>
         </is>
       </c>
       <c r="N150" t="inlineStr">
@@ -13532,7 +13631,7 @@
       </c>
       <c r="M151" t="inlineStr">
         <is>
-          <t>C303</t>
+          <t>C203</t>
         </is>
       </c>
       <c r="N151" t="inlineStr">
@@ -13608,7 +13707,7 @@
       </c>
       <c r="M152" t="inlineStr">
         <is>
-          <t>C304</t>
+          <t>C204</t>
         </is>
       </c>
       <c r="N152" t="inlineStr">
@@ -13684,7 +13783,7 @@
       </c>
       <c r="M153" t="inlineStr">
         <is>
-          <t>C305</t>
+          <t>C205</t>
         </is>
       </c>
       <c r="N153" t="inlineStr">
@@ -13732,15 +13831,19 @@
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H154" t="inlineStr">
         <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="I154" t="inlineStr"/>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
       <c r="J154" t="b">
         <v>0</v>
       </c>
@@ -13756,7 +13859,7 @@
       </c>
       <c r="M154" t="inlineStr">
         <is>
-          <t>C001</t>
+          <t>C302</t>
         </is>
       </c>
       <c r="N154" t="inlineStr">
@@ -13804,17 +13907,17 @@
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H155" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I155" t="inlineStr">
         <is>
-          <t>Projector</t>
+          <t>TV</t>
         </is>
       </c>
       <c r="J155" t="b">
@@ -13832,7 +13935,7 @@
       </c>
       <c r="M155" t="inlineStr">
         <is>
-          <t>C002</t>
+          <t>C303</t>
         </is>
       </c>
       <c r="N155" t="inlineStr">
@@ -13880,17 +13983,17 @@
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H156" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I156" t="inlineStr">
         <is>
-          <t>Projector</t>
+          <t>TV</t>
         </is>
       </c>
       <c r="J156" t="b">
@@ -13908,7 +14011,7 @@
       </c>
       <c r="M156" t="inlineStr">
         <is>
-          <t>C003</t>
+          <t>C304</t>
         </is>
       </c>
       <c r="N156" t="inlineStr">
@@ -14876,7 +14979,7 @@
       <c r="L169" t="inlineStr"/>
       <c r="M169" t="inlineStr">
         <is>
-          <t>L105</t>
+          <t>L206</t>
         </is>
       </c>
       <c r="N169" t="inlineStr">
@@ -15406,7 +15509,7 @@
       </c>
       <c r="I177" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J177" t="b">
@@ -15424,7 +15527,7 @@
       </c>
       <c r="M177" t="inlineStr">
         <is>
-          <t>C203</t>
+          <t>C101</t>
         </is>
       </c>
       <c r="N177" t="inlineStr">
@@ -15482,7 +15585,7 @@
       </c>
       <c r="I178" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J178" t="b">
@@ -15500,7 +15603,7 @@
       </c>
       <c r="M178" t="inlineStr">
         <is>
-          <t>C204</t>
+          <t>C102</t>
         </is>
       </c>
       <c r="N178" t="inlineStr">
@@ -15558,7 +15661,7 @@
       </c>
       <c r="I179" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J179" t="b">
@@ -15576,7 +15679,7 @@
       </c>
       <c r="M179" t="inlineStr">
         <is>
-          <t>C205</t>
+          <t>C104</t>
         </is>
       </c>
       <c r="N179" t="inlineStr">
@@ -15652,7 +15755,7 @@
       </c>
       <c r="M180" t="inlineStr">
         <is>
-          <t>C302</t>
+          <t>C202</t>
         </is>
       </c>
       <c r="N180" t="inlineStr">
@@ -15728,7 +15831,7 @@
       </c>
       <c r="M181" t="inlineStr">
         <is>
-          <t>C303</t>
+          <t>C203</t>
         </is>
       </c>
       <c r="N181" t="inlineStr">
@@ -15804,7 +15907,7 @@
       </c>
       <c r="M182" t="inlineStr">
         <is>
-          <t>C304</t>
+          <t>C204</t>
         </is>
       </c>
       <c r="N182" t="inlineStr">
@@ -15880,7 +15983,7 @@
       </c>
       <c r="M183" t="inlineStr">
         <is>
-          <t>C305</t>
+          <t>C205</t>
         </is>
       </c>
       <c r="N183" t="inlineStr">
@@ -15928,15 +16031,19 @@
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H184" t="inlineStr">
         <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="I184" t="inlineStr"/>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="I184" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
       <c r="J184" t="b">
         <v>0</v>
       </c>
@@ -15952,7 +16059,7 @@
       </c>
       <c r="M184" t="inlineStr">
         <is>
-          <t>C001</t>
+          <t>C302</t>
         </is>
       </c>
       <c r="N184" t="inlineStr">
@@ -16000,17 +16107,17 @@
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H185" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I185" t="inlineStr">
         <is>
-          <t>Projector</t>
+          <t>TV</t>
         </is>
       </c>
       <c r="J185" t="b">
@@ -16028,7 +16135,7 @@
       </c>
       <c r="M185" t="inlineStr">
         <is>
-          <t>C002</t>
+          <t>C303</t>
         </is>
       </c>
       <c r="N185" t="inlineStr">
@@ -16076,17 +16183,17 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H186" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I186" t="inlineStr">
         <is>
-          <t>Projector</t>
+          <t>TV</t>
         </is>
       </c>
       <c r="J186" t="b">
@@ -16104,7 +16211,7 @@
       </c>
       <c r="M186" t="inlineStr">
         <is>
-          <t>C003</t>
+          <t>C304</t>
         </is>
       </c>
       <c r="N186" t="inlineStr">
@@ -16238,7 +16345,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>C004, C101, C203</t>
+          <t>C004, C101</t>
         </is>
       </c>
     </row>
@@ -16255,7 +16362,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>C102, C204</t>
+          <t>C102</t>
         </is>
       </c>
     </row>
@@ -16272,7 +16379,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>C104, C205</t>
+          <t>C104</t>
         </is>
       </c>
     </row>
@@ -16289,7 +16396,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>C202, C302</t>
+          <t>C202</t>
         </is>
       </c>
     </row>
@@ -16306,7 +16413,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>C203, C303</t>
+          <t>C203</t>
         </is>
       </c>
     </row>
@@ -16323,7 +16430,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>C204, C304</t>
+          <t>C204</t>
         </is>
       </c>
     </row>
@@ -16340,7 +16447,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>C205, C305</t>
+          <t>C205</t>
         </is>
       </c>
     </row>
@@ -16357,7 +16464,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>C001, C302</t>
+          <t>C302</t>
         </is>
       </c>
     </row>
@@ -16374,7 +16481,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>C002, C303</t>
+          <t>C303</t>
         </is>
       </c>
     </row>
@@ -16391,7 +16498,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>C003, C304</t>
+          <t>C304</t>
         </is>
       </c>
     </row>
@@ -16606,7 +16713,7 @@
       </c>
       <c r="D6" s="14" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L206]</t>
+          <t>EC161 (Lab) [L105]</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -16639,7 +16746,7 @@
       </c>
       <c r="D7" s="14" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L206]</t>
+          <t>EC161 (Lab) [L105]</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -17657,7 +17764,7 @@
       </c>
       <c r="D6" s="14" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L105]</t>
+          <t>EC161 (Lab) [L206]</t>
         </is>
       </c>
       <c r="E6" s="11" t="inlineStr">
@@ -17690,7 +17797,7 @@
       </c>
       <c r="D7" s="14" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L105]</t>
+          <t>EC161 (Lab) [L206]</t>
         </is>
       </c>
       <c r="E7" s="11" t="inlineStr">
@@ -20876,7 +20983,7 @@
       </c>
       <c r="D8" s="14" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L206]</t>
+          <t>EC161 (Lab) [L105]</t>
         </is>
       </c>
       <c r="E8" s="8" t="inlineStr">
@@ -20909,7 +21016,7 @@
       </c>
       <c r="D9" s="14" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L206]</t>
+          <t>EC161 (Lab) [L105]</t>
         </is>
       </c>
       <c r="E9" s="8" t="inlineStr">
@@ -21927,7 +22034,7 @@
       </c>
       <c r="D8" s="14" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L105]</t>
+          <t>EC161 (Lab) [L206]</t>
         </is>
       </c>
       <c r="E8" s="8" t="inlineStr">
@@ -21960,7 +22067,7 @@
       </c>
       <c r="D9" s="14" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L105]</t>
+          <t>EC161 (Lab) [L206]</t>
         </is>
       </c>
       <c r="E9" s="8" t="inlineStr">
@@ -22797,7 +22904,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CS161 [C305]</t>
+          <t>CS161 [C102]</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -22824,7 +22931,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>CS161 [C305]</t>
+          <t>CS161 [C102]</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -22888,7 +22995,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [L107]</t>
+          <t>CS161 (Lab) [L207]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -22920,7 +23027,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [L208]</t>
+          <t>CS161 (Lab) [L207]</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -22952,7 +23059,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>HS161 [C304]</t>
+          <t>HS161 [C102]</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -22962,7 +23069,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L206]</t>
+          <t>EC161 (Lab) [L105]</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -22994,7 +23101,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L206]</t>
+          <t>EC161 (Lab) [L105]</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -23096,27 +23203,27 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Course Name [L406]</t>
+          <t>Course Name [C302]</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>L-T-P-S-C [L406]</t>
+          <t>L-T-P-S-C [C302]</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Term Type [L406]</t>
+          <t>Term Type [C302]</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Lectures Hrs [L406]</t>
+          <t>Lectures Hrs [C302]</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Tutorials Hrs [L406]</t>
+          <t>Tutorials Hrs [C302]</t>
         </is>
       </c>
     </row>
@@ -23344,27 +23451,27 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Course [L406]</t>
+          <t>Course [C302]</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Course Code [L406]</t>
+          <t>Course Code [C302]</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Lecture Slot - Classroom [L406]</t>
+          <t>Lecture Slot - Classroom [C302]</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Tutorial Slot - Classroom [L406]</t>
+          <t>Tutorial Slot - Classroom [C302]</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>L-T-P-S-C [L406]</t>
+          <t>L-T-P-S-C [C302]</t>
         </is>
       </c>
     </row>
@@ -23784,7 +23891,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CS161 [C204]</t>
+          <t>CS161 [C104]</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -23811,12 +23918,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>CS161 [C204]</t>
+          <t>CS161 [C104]</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>HS161 [C205]</t>
+          <t>HS161 [C104]</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -23875,7 +23982,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [L107]</t>
+          <t>CS161 (Lab) [L207]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -23907,7 +24014,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [C004]</t>
+          <t>CS161 (Lab) [L207]</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -23939,7 +24046,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>HS161 [C305]</t>
+          <t>HS161 [C104]</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -23949,7 +24056,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L105]</t>
+          <t>EC161 (Lab) [L206]</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -23981,7 +24088,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L105]</t>
+          <t>EC161 (Lab) [L206]</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -24083,27 +24190,27 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Course Name [L408]</t>
+          <t>Course Name [C303]</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>L-T-P-S-C [L408]</t>
+          <t>L-T-P-S-C [C303]</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Term Type [L408]</t>
+          <t>Term Type [C303]</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Lectures Hrs [L407]</t>
+          <t>Lectures Hrs [C303]</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Tutorials Hrs [L407]</t>
+          <t>Tutorials Hrs [C303]</t>
         </is>
       </c>
     </row>
@@ -24331,27 +24438,27 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Course [L408]</t>
+          <t>Course [C303]</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Course Code [L408]</t>
+          <t>Course Code [C303]</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Lecture Slot - Classroom [L408]</t>
+          <t>Lecture Slot - Classroom [C303]</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Tutorial Slot - Classroom [L408]</t>
+          <t>Tutorial Slot - Classroom [C303]</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>L-T-P-S-C [L408]</t>
+          <t>L-T-P-S-C [C303]</t>
         </is>
       </c>
     </row>

</xml_diff>